<commit_message>
Working text and country name boxes! :) :)
</commit_message>
<xml_diff>
--- a/pleasework.xlsx
+++ b/pleasework.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="291" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -815,6 +815,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -898,8 +899,8 @@
   </sheetPr>
   <dimension ref="A1:E258"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A255" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -937,8 +938,8 @@
         <v>66</v>
       </c>
       <c r="D2" s="0" t="n">
-        <f aca="false">1470* (180 + C2) / 360</f>
-        <v>1004.5</v>
+        <f aca="false">1470* (185 + C2) / 360</f>
+        <v>1024.91666666667</v>
       </c>
       <c r="E2" s="0" t="n">
         <f aca="false">735 * (90 - B2) / 180</f>
@@ -956,8 +957,8 @@
         <v>20</v>
       </c>
       <c r="D3" s="0" t="n">
-        <f aca="false">1470* (180 + C3) / 360</f>
-        <v>816.666666666667</v>
+        <f aca="false">1470* (185 + C3) / 360</f>
+        <v>837.083333333333</v>
       </c>
       <c r="E3" s="0" t="n">
         <f aca="false">735 * (90 - B3) / 180</f>
@@ -975,8 +976,8 @@
         <v>3</v>
       </c>
       <c r="D4" s="0" t="n">
-        <f aca="false">1470* (180 + C4) / 360</f>
-        <v>747.25</v>
+        <f aca="false">1470* (185 + C4) / 360</f>
+        <v>767.666666666667</v>
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">735 * (90 - B4) / 180</f>
@@ -994,8 +995,8 @@
         <v>-170</v>
       </c>
       <c r="D5" s="0" t="n">
-        <f aca="false">1470* (180 + C5) / 360</f>
-        <v>40.8333333333333</v>
+        <f aca="false">1470* (185 + C5) / 360</f>
+        <v>61.25</v>
       </c>
       <c r="E5" s="0" t="n">
         <f aca="false">735 * (90 - B5) / 180</f>
@@ -1013,8 +1014,8 @@
         <v>1.5</v>
       </c>
       <c r="D6" s="0" t="n">
-        <f aca="false">1470* (180 + C6) / 360</f>
-        <v>741.125</v>
+        <f aca="false">1470* (185 + C6) / 360</f>
+        <v>761.541666666667</v>
       </c>
       <c r="E6" s="0" t="n">
         <f aca="false">735 * (90 - B6) / 180</f>
@@ -1032,8 +1033,8 @@
         <v>18.5</v>
       </c>
       <c r="D7" s="0" t="n">
-        <f aca="false">1470* (180 + C7) / 360</f>
-        <v>810.541666666667</v>
+        <f aca="false">1470* (185 + C7) / 360</f>
+        <v>830.958333333333</v>
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">735 * (90 - B7) / 180</f>
@@ -1051,8 +1052,8 @@
         <v>-63.05</v>
       </c>
       <c r="D8" s="0" t="n">
-        <f aca="false">1470* (180 + C8) / 360</f>
-        <v>477.545833333333</v>
+        <f aca="false">1470* (185 + C8) / 360</f>
+        <v>497.9625</v>
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">735 * (90 - B8) / 180</f>
@@ -1070,8 +1071,8 @@
         <v>-61.8</v>
       </c>
       <c r="D9" s="0" t="n">
-        <f aca="false">1470* (180 + C9) / 360</f>
-        <v>482.65</v>
+        <f aca="false">1470* (185 + C9) / 360</f>
+        <v>503.066666666667</v>
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">735 * (90 - B9) / 180</f>
@@ -1089,8 +1090,8 @@
         <v>-64</v>
       </c>
       <c r="D10" s="0" t="n">
-        <f aca="false">1470* (180 + C10) / 360</f>
-        <v>473.666666666667</v>
+        <f aca="false">1470* (185 + C10) / 360</f>
+        <v>494.083333333333</v>
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">735 * (90 - B10) / 180</f>
@@ -1108,8 +1109,8 @@
         <v>45</v>
       </c>
       <c r="D11" s="0" t="n">
-        <f aca="false">1470* (180 + C11) / 360</f>
-        <v>918.75</v>
+        <f aca="false">1470* (185 + C11) / 360</f>
+        <v>939.166666666667</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">735 * (90 - B11) / 180</f>
@@ -1127,8 +1128,8 @@
         <v>-69.966667</v>
       </c>
       <c r="D12" s="0" t="n">
-        <f aca="false">1470* (180 + C12) / 360</f>
-        <v>449.302776416667</v>
+        <f aca="false">1470* (185 + C12) / 360</f>
+        <v>469.719443083333</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">735 * (90 - B12) / 180</f>
@@ -1146,8 +1147,8 @@
         <v>-5.7</v>
       </c>
       <c r="D13" s="0" t="n">
-        <f aca="false">1470* (180 + C13) / 360</f>
-        <v>711.725</v>
+        <f aca="false">1470* (185 + C13) / 360</f>
+        <v>732.141666666667</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">735 * (90 - B13) / 180</f>
@@ -1165,8 +1166,8 @@
         <v>123.333333</v>
       </c>
       <c r="D14" s="0" t="n">
-        <f aca="false">1470* (180 + C14) / 360</f>
-        <v>1238.61110975</v>
+        <f aca="false">1470* (185 + C14) / 360</f>
+        <v>1259.02777641667</v>
       </c>
       <c r="E14" s="0" t="n">
         <f aca="false">735 * (90 - B14) / 180</f>
@@ -1184,8 +1185,8 @@
         <v>135</v>
       </c>
       <c r="D15" s="0" t="n">
-        <f aca="false">1470* (180 + C15) / 360</f>
-        <v>1286.25</v>
+        <f aca="false">1470* (185 + C15) / 360</f>
+        <v>1306.66666666667</v>
       </c>
       <c r="E15" s="0" t="n">
         <f aca="false">735 * (90 - B15) / 180</f>
@@ -1203,8 +1204,8 @@
         <v>13.333333</v>
       </c>
       <c r="D16" s="0" t="n">
-        <f aca="false">1470* (180 + C16) / 360</f>
-        <v>789.444443083333</v>
+        <f aca="false">1470* (185 + C16) / 360</f>
+        <v>809.86110975</v>
       </c>
       <c r="E16" s="0" t="n">
         <f aca="false">735 * (90 - B16) / 180</f>
@@ -1222,8 +1223,8 @@
         <v>47.5</v>
       </c>
       <c r="D17" s="0" t="n">
-        <f aca="false">1470* (180 + C17) / 360</f>
-        <v>928.958333333333</v>
+        <f aca="false">1470* (185 + C17) / 360</f>
+        <v>949.375</v>
       </c>
       <c r="E17" s="0" t="n">
         <f aca="false">735 * (90 - B17) / 180</f>
@@ -1241,8 +1242,8 @@
         <v>-76</v>
       </c>
       <c r="D18" s="0" t="n">
-        <f aca="false">1470* (180 + C18) / 360</f>
-        <v>424.666666666667</v>
+        <f aca="false">1470* (185 + C18) / 360</f>
+        <v>445.083333333333</v>
       </c>
       <c r="E18" s="0" t="n">
         <f aca="false">735 * (90 - B18) / 180</f>
@@ -1260,8 +1261,8 @@
         <v>50.5</v>
       </c>
       <c r="D19" s="0" t="n">
-        <f aca="false">1470* (180 + C19) / 360</f>
-        <v>941.208333333333</v>
+        <f aca="false">1470* (185 + C19) / 360</f>
+        <v>961.625</v>
       </c>
       <c r="E19" s="0" t="n">
         <f aca="false">735 * (90 - B19) / 180</f>
@@ -1279,8 +1280,8 @@
         <v>90</v>
       </c>
       <c r="D20" s="0" t="n">
-        <f aca="false">1470* (180 + C20) / 360</f>
-        <v>1102.5</v>
+        <f aca="false">1470* (185 + C20) / 360</f>
+        <v>1122.91666666667</v>
       </c>
       <c r="E20" s="0" t="n">
         <f aca="false">735 * (90 - B20) / 180</f>
@@ -1298,8 +1299,8 @@
         <v>-59.533333</v>
       </c>
       <c r="D21" s="0" t="n">
-        <f aca="false">1470* (180 + C21) / 360</f>
-        <v>491.905556916667</v>
+        <f aca="false">1470* (185 + C21) / 360</f>
+        <v>512.322223583333</v>
       </c>
       <c r="E21" s="0" t="n">
         <f aca="false">735 * (90 - B21) / 180</f>
@@ -1317,8 +1318,8 @@
         <v>39.7</v>
       </c>
       <c r="D22" s="0" t="n">
-        <f aca="false">1470* (180 + C22) / 360</f>
-        <v>897.108333333333</v>
+        <f aca="false">1470* (185 + C22) / 360</f>
+        <v>917.525</v>
       </c>
       <c r="E22" s="0" t="n">
         <f aca="false">735 * (90 - B22) / 180</f>
@@ -1336,8 +1337,8 @@
         <v>28</v>
       </c>
       <c r="D23" s="0" t="n">
-        <f aca="false">1470* (180 + C23) / 360</f>
-        <v>849.333333333333</v>
+        <f aca="false">1470* (185 + C23) / 360</f>
+        <v>869.75</v>
       </c>
       <c r="E23" s="0" t="n">
         <f aca="false">735 * (90 - B23) / 180</f>
@@ -1355,8 +1356,8 @@
         <v>4</v>
       </c>
       <c r="D24" s="0" t="n">
-        <f aca="false">1470* (180 + C24) / 360</f>
-        <v>751.333333333333</v>
+        <f aca="false">1470* (185 + C24) / 360</f>
+        <v>771.75</v>
       </c>
       <c r="E24" s="0" t="n">
         <f aca="false">735 * (90 - B24) / 180</f>
@@ -1374,8 +1375,8 @@
         <v>-88.75</v>
       </c>
       <c r="D25" s="0" t="n">
-        <f aca="false">1470* (180 + C25) / 360</f>
-        <v>372.604166666667</v>
+        <f aca="false">1470* (185 + C25) / 360</f>
+        <v>393.020833333333</v>
       </c>
       <c r="E25" s="0" t="n">
         <f aca="false">735 * (90 - B25) / 180</f>
@@ -1393,8 +1394,8 @@
         <v>2.25</v>
       </c>
       <c r="D26" s="0" t="n">
-        <f aca="false">1470* (180 + C26) / 360</f>
-        <v>744.1875</v>
+        <f aca="false">1470* (185 + C26) / 360</f>
+        <v>764.604166666667</v>
       </c>
       <c r="E26" s="0" t="n">
         <f aca="false">735 * (90 - B26) / 180</f>
@@ -1412,8 +1413,8 @@
         <v>-64.75</v>
       </c>
       <c r="D27" s="0" t="n">
-        <f aca="false">1470* (180 + C27) / 360</f>
-        <v>470.604166666667</v>
+        <f aca="false">1470* (185 + C27) / 360</f>
+        <v>491.020833333333</v>
       </c>
       <c r="E27" s="0" t="n">
         <f aca="false">735 * (90 - B27) / 180</f>
@@ -1431,8 +1432,8 @@
         <v>90.5</v>
       </c>
       <c r="D28" s="0" t="n">
-        <f aca="false">1470* (180 + C28) / 360</f>
-        <v>1104.54166666667</v>
+        <f aca="false">1470* (185 + C28) / 360</f>
+        <v>1124.95833333333</v>
       </c>
       <c r="E28" s="0" t="n">
         <f aca="false">735 * (90 - B28) / 180</f>
@@ -1450,8 +1451,8 @@
         <v>-65</v>
       </c>
       <c r="D29" s="0" t="n">
-        <f aca="false">1470* (180 + C29) / 360</f>
-        <v>469.583333333333</v>
+        <f aca="false">1470* (185 + C29) / 360</f>
+        <v>490</v>
       </c>
       <c r="E29" s="0" t="n">
         <f aca="false">735 * (90 - B29) / 180</f>
@@ -1469,8 +1470,8 @@
         <v>-68.25</v>
       </c>
       <c r="D30" s="0" t="n">
-        <f aca="false">1470* (180 + C30) / 360</f>
-        <v>456.3125</v>
+        <f aca="false">1470* (185 + C30) / 360</f>
+        <v>476.729166666667</v>
       </c>
       <c r="E30" s="0" t="n">
         <f aca="false">735 * (90 - B30) / 180</f>
@@ -1488,8 +1489,8 @@
         <v>17.833333</v>
       </c>
       <c r="D31" s="0" t="n">
-        <f aca="false">1470* (180 + C31) / 360</f>
-        <v>807.819443083333</v>
+        <f aca="false">1470* (185 + C31) / 360</f>
+        <v>828.23610975</v>
       </c>
       <c r="E31" s="0" t="n">
         <f aca="false">735 * (90 - B31) / 180</f>
@@ -1507,8 +1508,8 @@
         <v>24</v>
       </c>
       <c r="D32" s="0" t="n">
-        <f aca="false">1470* (180 + C32) / 360</f>
-        <v>833</v>
+        <f aca="false">1470* (185 + C32) / 360</f>
+        <v>853.416666666667</v>
       </c>
       <c r="E32" s="0" t="n">
         <f aca="false">735 * (90 - B32) / 180</f>
@@ -1526,8 +1527,8 @@
         <v>3.4</v>
       </c>
       <c r="D33" s="0" t="n">
-        <f aca="false">1470* (180 + C33) / 360</f>
-        <v>748.883333333333</v>
+        <f aca="false">1470* (185 + C33) / 360</f>
+        <v>769.3</v>
       </c>
       <c r="E33" s="0" t="n">
         <f aca="false">735 * (90 - B33) / 180</f>
@@ -1545,8 +1546,8 @@
         <v>-55</v>
       </c>
       <c r="D34" s="0" t="n">
-        <f aca="false">1470* (180 + C34) / 360</f>
-        <v>510.416666666667</v>
+        <f aca="false">1470* (185 + C34) / 360</f>
+        <v>530.833333333333</v>
       </c>
       <c r="E34" s="0" t="n">
         <f aca="false">735 * (90 - B34) / 180</f>
@@ -1564,8 +1565,8 @@
         <v>72</v>
       </c>
       <c r="D35" s="0" t="n">
-        <f aca="false">1470* (180 + C35) / 360</f>
-        <v>1029</v>
+        <f aca="false">1470* (185 + C35) / 360</f>
+        <v>1049.41666666667</v>
       </c>
       <c r="E35" s="0" t="n">
         <f aca="false">735 * (90 - B35) / 180</f>
@@ -1583,8 +1584,8 @@
         <v>-64.5</v>
       </c>
       <c r="D36" s="0" t="n">
-        <f aca="false">1470* (180 + C36) / 360</f>
-        <v>471.625</v>
+        <f aca="false">1470* (185 + C36) / 360</f>
+        <v>492.041666666667</v>
       </c>
       <c r="E36" s="0" t="n">
         <f aca="false">735 * (90 - B36) / 180</f>
@@ -1602,8 +1603,8 @@
         <v>114.666667</v>
       </c>
       <c r="D37" s="0" t="n">
-        <f aca="false">1470* (180 + C37) / 360</f>
-        <v>1203.22222358333</v>
+        <f aca="false">1470* (185 + C37) / 360</f>
+        <v>1223.63889025</v>
       </c>
       <c r="E37" s="0" t="n">
         <f aca="false">735 * (90 - B37) / 180</f>
@@ -1621,8 +1622,8 @@
         <v>25</v>
       </c>
       <c r="D38" s="0" t="n">
-        <f aca="false">1470* (180 + C38) / 360</f>
-        <v>837.083333333333</v>
+        <f aca="false">1470* (185 + C38) / 360</f>
+        <v>857.5</v>
       </c>
       <c r="E38" s="0" t="n">
         <f aca="false">735 * (90 - B38) / 180</f>
@@ -1640,8 +1641,8 @@
         <v>-2</v>
       </c>
       <c r="D39" s="0" t="n">
-        <f aca="false">1470* (180 + C39) / 360</f>
-        <v>726.833333333333</v>
+        <f aca="false">1470* (185 + C39) / 360</f>
+        <v>747.25</v>
       </c>
       <c r="E39" s="0" t="n">
         <f aca="false">735 * (90 - B39) / 180</f>
@@ -1659,8 +1660,8 @@
         <v>98</v>
       </c>
       <c r="D40" s="0" t="n">
-        <f aca="false">1470* (180 + C40) / 360</f>
-        <v>1135.16666666667</v>
+        <f aca="false">1470* (185 + C40) / 360</f>
+        <v>1155.58333333333</v>
       </c>
       <c r="E40" s="0" t="n">
         <f aca="false">735 * (90 - B40) / 180</f>
@@ -1678,8 +1679,8 @@
         <v>30</v>
       </c>
       <c r="D41" s="0" t="n">
-        <f aca="false">1470* (180 + C41) / 360</f>
-        <v>857.5</v>
+        <f aca="false">1470* (185 + C41) / 360</f>
+        <v>877.916666666667</v>
       </c>
       <c r="E41" s="0" t="n">
         <f aca="false">735 * (90 - B41) / 180</f>
@@ -1697,8 +1698,8 @@
         <v>105</v>
       </c>
       <c r="D42" s="0" t="n">
-        <f aca="false">1470* (180 + C42) / 360</f>
-        <v>1163.75</v>
+        <f aca="false">1470* (185 + C42) / 360</f>
+        <v>1184.16666666667</v>
       </c>
       <c r="E42" s="0" t="n">
         <f aca="false">735 * (90 - B42) / 180</f>
@@ -1716,8 +1717,8 @@
         <v>12</v>
       </c>
       <c r="D43" s="0" t="n">
-        <f aca="false">1470* (180 + C43) / 360</f>
-        <v>784</v>
+        <f aca="false">1470* (185 + C43) / 360</f>
+        <v>804.416666666667</v>
       </c>
       <c r="E43" s="0" t="n">
         <f aca="false">735 * (90 - B43) / 180</f>
@@ -1735,8 +1736,8 @@
         <v>-96</v>
       </c>
       <c r="D44" s="0" t="n">
-        <f aca="false">1470* (180 + C44) / 360</f>
-        <v>343</v>
+        <f aca="false">1470* (185 + C44) / 360</f>
+        <v>363.416666666667</v>
       </c>
       <c r="E44" s="0" t="n">
         <f aca="false">735 * (90 - B44) / 180</f>
@@ -1754,8 +1755,8 @@
         <v>-24</v>
       </c>
       <c r="D45" s="0" t="n">
-        <f aca="false">1470* (180 + C45) / 360</f>
-        <v>637</v>
+        <f aca="false">1470* (185 + C45) / 360</f>
+        <v>657.416666666667</v>
       </c>
       <c r="E45" s="0" t="n">
         <f aca="false">735 * (90 - B45) / 180</f>
@@ -1773,8 +1774,8 @@
         <v>-80.666667</v>
       </c>
       <c r="D46" s="0" t="n">
-        <f aca="false">1470* (180 + C46) / 360</f>
-        <v>405.61110975</v>
+        <f aca="false">1470* (185 + C46) / 360</f>
+        <v>426.027776416667</v>
       </c>
       <c r="E46" s="0" t="n">
         <f aca="false">735 * (90 - B46) / 180</f>
@@ -1792,8 +1793,8 @@
         <v>21</v>
       </c>
       <c r="D47" s="0" t="n">
-        <f aca="false">1470* (180 + C47) / 360</f>
-        <v>820.75</v>
+        <f aca="false">1470* (185 + C47) / 360</f>
+        <v>841.166666666667</v>
       </c>
       <c r="E47" s="0" t="n">
         <f aca="false">735 * (90 - B47) / 180</f>
@@ -1811,8 +1812,8 @@
         <v>19</v>
       </c>
       <c r="D48" s="0" t="n">
-        <f aca="false">1470* (180 + C48) / 360</f>
-        <v>812.583333333333</v>
+        <f aca="false">1470* (185 + C48) / 360</f>
+        <v>833</v>
       </c>
       <c r="E48" s="0" t="n">
         <f aca="false">735 * (90 - B48) / 180</f>
@@ -1830,8 +1831,8 @@
         <v>-71</v>
       </c>
       <c r="D49" s="0" t="n">
-        <f aca="false">1470* (180 + C49) / 360</f>
-        <v>445.083333333333</v>
+        <f aca="false">1470* (185 + C49) / 360</f>
+        <v>465.5</v>
       </c>
       <c r="E49" s="0" t="n">
         <f aca="false">735 * (90 - B49) / 180</f>
@@ -1849,8 +1850,8 @@
         <v>105</v>
       </c>
       <c r="D50" s="0" t="n">
-        <f aca="false">1470* (180 + C50) / 360</f>
-        <v>1163.75</v>
+        <f aca="false">1470* (185 + C50) / 360</f>
+        <v>1184.16666666667</v>
       </c>
       <c r="E50" s="0" t="n">
         <f aca="false">735 * (90 - B50) / 180</f>
@@ -1868,8 +1869,8 @@
         <v>105.666667</v>
       </c>
       <c r="D51" s="0" t="n">
-        <f aca="false">1470* (180 + C51) / 360</f>
-        <v>1166.47222358333</v>
+        <f aca="false">1470* (185 + C51) / 360</f>
+        <v>1186.88889025</v>
       </c>
       <c r="E51" s="0" t="n">
         <f aca="false">735 * (90 - B51) / 180</f>
@@ -1887,8 +1888,8 @@
         <v>-109.216667</v>
       </c>
       <c r="D52" s="0" t="n">
-        <f aca="false">1470* (180 + C52) / 360</f>
-        <v>289.031943083333</v>
+        <f aca="false">1470* (185 + C52) / 360</f>
+        <v>309.44860975</v>
       </c>
       <c r="E52" s="0" t="n">
         <f aca="false">735 * (90 - B52) / 180</f>
@@ -1906,8 +1907,8 @@
         <v>96.833333</v>
       </c>
       <c r="D53" s="0" t="n">
-        <f aca="false">1470* (180 + C53) / 360</f>
-        <v>1130.40277641667</v>
+        <f aca="false">1470* (185 + C53) / 360</f>
+        <v>1150.81944308333</v>
       </c>
       <c r="E53" s="0" t="n">
         <f aca="false">735 * (90 - B53) / 180</f>
@@ -1925,8 +1926,8 @@
         <v>-72</v>
       </c>
       <c r="D54" s="0" t="n">
-        <f aca="false">1470* (180 + C54) / 360</f>
-        <v>441</v>
+        <f aca="false">1470* (185 + C54) / 360</f>
+        <v>461.416666666667</v>
       </c>
       <c r="E54" s="0" t="n">
         <f aca="false">735 * (90 - B54) / 180</f>
@@ -1944,8 +1945,8 @@
         <v>44.25</v>
       </c>
       <c r="D55" s="0" t="n">
-        <f aca="false">1470* (180 + C55) / 360</f>
-        <v>915.6875</v>
+        <f aca="false">1470* (185 + C55) / 360</f>
+        <v>936.104166666667</v>
       </c>
       <c r="E55" s="0" t="n">
         <f aca="false">735 * (90 - B55) / 180</f>
@@ -1963,8 +1964,8 @@
         <v>-161.583333</v>
       </c>
       <c r="D56" s="0" t="n">
-        <f aca="false">1470* (180 + C56) / 360</f>
-        <v>75.20139025</v>
+        <f aca="false">1470* (185 + C56) / 360</f>
+        <v>95.6180569166666</v>
       </c>
       <c r="E56" s="0" t="n">
         <f aca="false">735 * (90 - B56) / 180</f>
@@ -1982,8 +1983,8 @@
         <v>151</v>
       </c>
       <c r="D57" s="0" t="n">
-        <f aca="false">1470* (180 + C57) / 360</f>
-        <v>1351.58333333333</v>
+        <f aca="false">1470* (185 + C57) / 360</f>
+        <v>1372</v>
       </c>
       <c r="E57" s="0" t="n">
         <f aca="false">735 * (90 - B57) / 180</f>
@@ -2001,8 +2002,8 @@
         <v>-84</v>
       </c>
       <c r="D58" s="0" t="n">
-        <f aca="false">1470* (180 + C58) / 360</f>
-        <v>392</v>
+        <f aca="false">1470* (185 + C58) / 360</f>
+        <v>412.416666666667</v>
       </c>
       <c r="E58" s="0" t="n">
         <f aca="false">735 * (90 - B58) / 180</f>
@@ -2020,8 +2021,8 @@
         <v>-5</v>
       </c>
       <c r="D59" s="0" t="n">
-        <f aca="false">1470* (180 + C59) / 360</f>
-        <v>714.583333333333</v>
+        <f aca="false">1470* (185 + C59) / 360</f>
+        <v>735</v>
       </c>
       <c r="E59" s="0" t="n">
         <f aca="false">735 * (90 - B59) / 180</f>
@@ -2039,8 +2040,8 @@
         <v>15.5</v>
       </c>
       <c r="D60" s="0" t="n">
-        <f aca="false">1470* (180 + C60) / 360</f>
-        <v>798.291666666667</v>
+        <f aca="false">1470* (185 + C60) / 360</f>
+        <v>818.708333333333</v>
       </c>
       <c r="E60" s="0" t="n">
         <f aca="false">735 * (90 - B60) / 180</f>
@@ -2058,8 +2059,8 @@
         <v>-79.5</v>
       </c>
       <c r="D61" s="0" t="n">
-        <f aca="false">1470* (180 + C61) / 360</f>
-        <v>410.375</v>
+        <f aca="false">1470* (185 + C61) / 360</f>
+        <v>430.791666666667</v>
       </c>
       <c r="E61" s="0" t="n">
         <f aca="false">735 * (90 - B61) / 180</f>
@@ -2077,8 +2078,8 @@
         <v>-69</v>
       </c>
       <c r="D62" s="0" t="n">
-        <f aca="false">1470* (180 + C62) / 360</f>
-        <v>453.25</v>
+        <f aca="false">1470* (185 + C62) / 360</f>
+        <v>473.666666666667</v>
       </c>
       <c r="E62" s="0" t="n">
         <f aca="false">735 * (90 - B62) / 180</f>
@@ -2096,8 +2097,8 @@
         <v>33</v>
       </c>
       <c r="D63" s="0" t="n">
-        <f aca="false">1470* (180 + C63) / 360</f>
-        <v>869.75</v>
+        <f aca="false">1470* (185 + C63) / 360</f>
+        <v>890.166666666667</v>
       </c>
       <c r="E63" s="0" t="n">
         <f aca="false">735 * (90 - B63) / 180</f>
@@ -2115,8 +2116,8 @@
         <v>15</v>
       </c>
       <c r="D64" s="0" t="n">
-        <f aca="false">1470* (180 + C64) / 360</f>
-        <v>796.25</v>
+        <f aca="false">1470* (185 + C64) / 360</f>
+        <v>816.666666666667</v>
       </c>
       <c r="E64" s="0" t="n">
         <f aca="false">735 * (90 - B64) / 180</f>
@@ -2134,8 +2135,8 @@
         <v>25</v>
       </c>
       <c r="D65" s="0" t="n">
-        <f aca="false">1470* (180 + C65) / 360</f>
-        <v>837.083333333333</v>
+        <f aca="false">1470* (185 + C65) / 360</f>
+        <v>857.5</v>
       </c>
       <c r="E65" s="0" t="n">
         <f aca="false">735 * (90 - B65) / 180</f>
@@ -2153,8 +2154,8 @@
         <v>10</v>
       </c>
       <c r="D66" s="0" t="n">
-        <f aca="false">1470* (180 + C66) / 360</f>
-        <v>775.833333333333</v>
+        <f aca="false">1470* (185 + C66) / 360</f>
+        <v>796.25</v>
       </c>
       <c r="E66" s="0" t="n">
         <f aca="false">735 * (90 - B66) / 180</f>
@@ -2172,8 +2173,8 @@
         <v>42.5</v>
       </c>
       <c r="D67" s="0" t="n">
-        <f aca="false">1470* (180 + C67) / 360</f>
-        <v>908.541666666667</v>
+        <f aca="false">1470* (185 + C67) / 360</f>
+        <v>928.958333333333</v>
       </c>
       <c r="E67" s="0" t="n">
         <f aca="false">735 * (90 - B67) / 180</f>
@@ -2191,8 +2192,8 @@
         <v>-61.333333</v>
       </c>
       <c r="D68" s="0" t="n">
-        <f aca="false">1470* (180 + C68) / 360</f>
-        <v>484.555556916667</v>
+        <f aca="false">1470* (185 + C68) / 360</f>
+        <v>504.972223583333</v>
       </c>
       <c r="E68" s="0" t="n">
         <f aca="false">735 * (90 - B68) / 180</f>
@@ -2210,8 +2211,8 @@
         <v>-70.666667</v>
       </c>
       <c r="D69" s="0" t="n">
-        <f aca="false">1470* (180 + C69) / 360</f>
-        <v>446.444443083333</v>
+        <f aca="false">1470* (185 + C69) / 360</f>
+        <v>466.86110975</v>
       </c>
       <c r="E69" s="0" t="n">
         <f aca="false">735 * (90 - B69) / 180</f>
@@ -2229,8 +2230,8 @@
         <v>-77.5</v>
       </c>
       <c r="D70" s="0" t="n">
-        <f aca="false">1470* (180 + C70) / 360</f>
-        <v>418.541666666667</v>
+        <f aca="false">1470* (185 + C70) / 360</f>
+        <v>438.958333333333</v>
       </c>
       <c r="E70" s="0" t="n">
         <f aca="false">735 * (90 - B70) / 180</f>
@@ -2248,8 +2249,8 @@
         <v>30</v>
       </c>
       <c r="D71" s="0" t="n">
-        <f aca="false">1470* (180 + C71) / 360</f>
-        <v>857.5</v>
+        <f aca="false">1470* (185 + C71) / 360</f>
+        <v>877.916666666667</v>
       </c>
       <c r="E71" s="0" t="n">
         <f aca="false">735 * (90 - B71) / 180</f>
@@ -2267,8 +2268,8 @@
         <v>-88.916667</v>
       </c>
       <c r="D72" s="0" t="n">
-        <f aca="false">1470* (180 + C72) / 360</f>
-        <v>371.92360975</v>
+        <f aca="false">1470* (185 + C72) / 360</f>
+        <v>392.340276416667</v>
       </c>
       <c r="E72" s="0" t="n">
         <f aca="false">735 * (90 - B72) / 180</f>
@@ -2286,8 +2287,8 @@
         <v>10</v>
       </c>
       <c r="D73" s="0" t="n">
-        <f aca="false">1470* (180 + C73) / 360</f>
-        <v>775.833333333333</v>
+        <f aca="false">1470* (185 + C73) / 360</f>
+        <v>796.25</v>
       </c>
       <c r="E73" s="0" t="n">
         <f aca="false">735 * (90 - B73) / 180</f>
@@ -2305,8 +2306,8 @@
         <v>39</v>
       </c>
       <c r="D74" s="0" t="n">
-        <f aca="false">1470* (180 + C74) / 360</f>
-        <v>894.25</v>
+        <f aca="false">1470* (185 + C74) / 360</f>
+        <v>914.666666666667</v>
       </c>
       <c r="E74" s="0" t="n">
         <f aca="false">735 * (90 - B74) / 180</f>
@@ -2324,8 +2325,8 @@
         <v>26</v>
       </c>
       <c r="D75" s="0" t="n">
-        <f aca="false">1470* (180 + C75) / 360</f>
-        <v>841.166666666667</v>
+        <f aca="false">1470* (185 + C75) / 360</f>
+        <v>861.583333333333</v>
       </c>
       <c r="E75" s="0" t="n">
         <f aca="false">735 * (90 - B75) / 180</f>
@@ -2343,8 +2344,8 @@
         <v>38</v>
       </c>
       <c r="D76" s="0" t="n">
-        <f aca="false">1470* (180 + C76) / 360</f>
-        <v>890.166666666667</v>
+        <f aca="false">1470* (185 + C76) / 360</f>
+        <v>910.583333333333</v>
       </c>
       <c r="E76" s="0" t="n">
         <f aca="false">735 * (90 - B76) / 180</f>
@@ -2362,8 +2363,8 @@
         <v>40.366667</v>
       </c>
       <c r="D77" s="0" t="n">
-        <f aca="false">1470* (180 + C77) / 360</f>
-        <v>899.830556916667</v>
+        <f aca="false">1470* (185 + C77) / 360</f>
+        <v>920.247223583333</v>
       </c>
       <c r="E77" s="0" t="n">
         <f aca="false">735 * (90 - B77) / 180</f>
@@ -2381,8 +2382,8 @@
         <v>-59.166667</v>
       </c>
       <c r="D78" s="0" t="n">
-        <f aca="false">1470* (180 + C78) / 360</f>
-        <v>493.402776416667</v>
+        <f aca="false">1470* (185 + C78) / 360</f>
+        <v>513.819443083334</v>
       </c>
       <c r="E78" s="0" t="n">
         <f aca="false">735 * (90 - B78) / 180</f>
@@ -2400,8 +2401,8 @@
         <v>-7</v>
       </c>
       <c r="D79" s="0" t="n">
-        <f aca="false">1470* (180 + C79) / 360</f>
-        <v>706.416666666667</v>
+        <f aca="false">1470* (185 + C79) / 360</f>
+        <v>726.833333333333</v>
       </c>
       <c r="E79" s="0" t="n">
         <f aca="false">735 * (90 - B79) / 180</f>
@@ -2419,8 +2420,8 @@
         <v>152</v>
       </c>
       <c r="D80" s="0" t="n">
-        <f aca="false">1470* (180 + C80) / 360</f>
-        <v>1355.66666666667</v>
+        <f aca="false">1470* (185 + C80) / 360</f>
+        <v>1376.08333333333</v>
       </c>
       <c r="E80" s="0" t="n">
         <f aca="false">735 * (90 - B80) / 180</f>
@@ -2438,8 +2439,8 @@
         <v>178</v>
       </c>
       <c r="D81" s="0" t="n">
-        <f aca="false">1470* (180 + C81) / 360</f>
-        <v>1461.83333333333</v>
+        <f aca="false">1470* (185 + C81) / 360</f>
+        <v>1482.25</v>
       </c>
       <c r="E81" s="0" t="n">
         <f aca="false">735 * (90 - B81) / 180</f>
@@ -2457,8 +2458,8 @@
         <v>26</v>
       </c>
       <c r="D82" s="0" t="n">
-        <f aca="false">1470* (180 + C82) / 360</f>
-        <v>841.166666666667</v>
+        <f aca="false">1470* (185 + C82) / 360</f>
+        <v>861.583333333333</v>
       </c>
       <c r="E82" s="0" t="n">
         <f aca="false">735 * (90 - B82) / 180</f>
@@ -2476,8 +2477,8 @@
         <v>2</v>
       </c>
       <c r="D83" s="0" t="n">
-        <f aca="false">1470* (180 + C83) / 360</f>
-        <v>743.166666666667</v>
+        <f aca="false">1470* (185 + C83) / 360</f>
+        <v>763.583333333333</v>
       </c>
       <c r="E83" s="0" t="n">
         <f aca="false">735 * (90 - B83) / 180</f>
@@ -2495,8 +2496,8 @@
         <v>-53</v>
       </c>
       <c r="D84" s="0" t="n">
-        <f aca="false">1470* (180 + C84) / 360</f>
-        <v>518.583333333333</v>
+        <f aca="false">1470* (185 + C84) / 360</f>
+        <v>539</v>
       </c>
       <c r="E84" s="0" t="n">
         <f aca="false">735 * (90 - B84) / 180</f>
@@ -2514,8 +2515,8 @@
         <v>-140</v>
       </c>
       <c r="D85" s="0" t="n">
-        <f aca="false">1470* (180 + C85) / 360</f>
-        <v>163.333333333333</v>
+        <f aca="false">1470* (185 + C85) / 360</f>
+        <v>183.75</v>
       </c>
       <c r="E85" s="0" t="n">
         <f aca="false">735 * (90 - B85) / 180</f>
@@ -2533,8 +2534,8 @@
         <v>67</v>
       </c>
       <c r="D86" s="0" t="n">
-        <f aca="false">1470* (180 + C86) / 360</f>
-        <v>1008.58333333333</v>
+        <f aca="false">1470* (185 + C86) / 360</f>
+        <v>1029</v>
       </c>
       <c r="E86" s="0" t="n">
         <f aca="false">735 * (90 - B86) / 180</f>
@@ -2552,8 +2553,8 @@
         <v>11.75</v>
       </c>
       <c r="D87" s="0" t="n">
-        <f aca="false">1470* (180 + C87) / 360</f>
-        <v>782.979166666667</v>
+        <f aca="false">1470* (185 + C87) / 360</f>
+        <v>803.395833333333</v>
       </c>
       <c r="E87" s="0" t="n">
         <f aca="false">735 * (90 - B87) / 180</f>
@@ -2571,8 +2572,8 @@
         <v>-15.5</v>
       </c>
       <c r="D88" s="0" t="n">
-        <f aca="false">1470* (180 + C88) / 360</f>
-        <v>671.708333333333</v>
+        <f aca="false">1470* (185 + C88) / 360</f>
+        <v>692.125</v>
       </c>
       <c r="E88" s="0" t="n">
         <f aca="false">735 * (90 - B88) / 180</f>
@@ -2590,8 +2591,8 @@
         <v>34.373398</v>
       </c>
       <c r="D89" s="0" t="n">
-        <f aca="false">1470* (180 + C89) / 360</f>
-        <v>875.358041833333</v>
+        <f aca="false">1470* (185 + C89) / 360</f>
+        <v>895.7747085</v>
       </c>
       <c r="E89" s="0" t="n">
         <f aca="false">735 * (90 - B89) / 180</f>
@@ -2609,8 +2610,8 @@
         <v>43.499905</v>
       </c>
       <c r="D90" s="0" t="n">
-        <f aca="false">1470* (180 + C90) / 360</f>
-        <v>912.624612083333</v>
+        <f aca="false">1470* (185 + C90) / 360</f>
+        <v>933.04127875</v>
       </c>
       <c r="E90" s="0" t="n">
         <f aca="false">735 * (90 - B90) / 180</f>
@@ -2628,8 +2629,8 @@
         <v>10.5</v>
       </c>
       <c r="D91" s="0" t="n">
-        <f aca="false">1470* (180 + C91) / 360</f>
-        <v>777.875</v>
+        <f aca="false">1470* (185 + C91) / 360</f>
+        <v>798.291666666667</v>
       </c>
       <c r="E91" s="0" t="n">
         <f aca="false">735 * (90 - B91) / 180</f>
@@ -2647,8 +2648,8 @@
         <v>-2</v>
       </c>
       <c r="D92" s="0" t="n">
-        <f aca="false">1470* (180 + C92) / 360</f>
-        <v>726.833333333333</v>
+        <f aca="false">1470* (185 + C92) / 360</f>
+        <v>747.25</v>
       </c>
       <c r="E92" s="0" t="n">
         <f aca="false">735 * (90 - B92) / 180</f>
@@ -2666,8 +2667,8 @@
         <v>-5.35</v>
       </c>
       <c r="D93" s="0" t="n">
-        <f aca="false">1470* (180 + C93) / 360</f>
-        <v>713.154166666667</v>
+        <f aca="false">1470* (185 + C93) / 360</f>
+        <v>733.570833333333</v>
       </c>
       <c r="E93" s="0" t="n">
         <f aca="false">735 * (90 - B93) / 180</f>
@@ -2685,8 +2686,8 @@
         <v>47.333333</v>
       </c>
       <c r="D94" s="0" t="n">
-        <f aca="false">1470* (180 + C94) / 360</f>
-        <v>928.277776416667</v>
+        <f aca="false">1470* (185 + C94) / 360</f>
+        <v>948.694443083333</v>
       </c>
       <c r="E94" s="0" t="n">
         <f aca="false">735 * (90 - B94) / 180</f>
@@ -2704,8 +2705,8 @@
         <v>22</v>
       </c>
       <c r="D95" s="0" t="n">
-        <f aca="false">1470* (180 + C95) / 360</f>
-        <v>824.833333333333</v>
+        <f aca="false">1470* (185 + C95) / 360</f>
+        <v>845.25</v>
       </c>
       <c r="E95" s="0" t="n">
         <f aca="false">735 * (90 - B95) / 180</f>
@@ -2723,8 +2724,8 @@
         <v>-40</v>
       </c>
       <c r="D96" s="0" t="n">
-        <f aca="false">1470* (180 + C96) / 360</f>
-        <v>571.666666666667</v>
+        <f aca="false">1470* (185 + C96) / 360</f>
+        <v>592.083333333333</v>
       </c>
       <c r="E96" s="0" t="n">
         <f aca="false">735 * (90 - B96) / 180</f>
@@ -2742,8 +2743,8 @@
         <v>-61.666667</v>
       </c>
       <c r="D97" s="0" t="n">
-        <f aca="false">1470* (180 + C97) / 360</f>
-        <v>483.194443083333</v>
+        <f aca="false">1470* (185 + C97) / 360</f>
+        <v>503.61110975</v>
       </c>
       <c r="E97" s="0" t="n">
         <f aca="false">735 * (90 - B97) / 180</f>
@@ -2761,8 +2762,8 @@
         <v>-61.583333</v>
       </c>
       <c r="D98" s="0" t="n">
-        <f aca="false">1470* (180 + C98) / 360</f>
-        <v>483.534723583333</v>
+        <f aca="false">1470* (185 + C98) / 360</f>
+        <v>503.95139025</v>
       </c>
       <c r="E98" s="0" t="n">
         <f aca="false">735 * (90 - B98) / 180</f>
@@ -2780,8 +2781,8 @@
         <v>144.7366667</v>
       </c>
       <c r="D99" s="0" t="n">
-        <f aca="false">1470* (180 + C99) / 360</f>
-        <v>1326.00805569167</v>
+        <f aca="false">1470* (185 + C99) / 360</f>
+        <v>1346.42472235833</v>
       </c>
       <c r="E99" s="0" t="n">
         <f aca="false">735 * (90 - B99) / 180</f>
@@ -2799,8 +2800,8 @@
         <v>-90.25</v>
       </c>
       <c r="D100" s="0" t="n">
-        <f aca="false">1470* (180 + C100) / 360</f>
-        <v>366.479166666667</v>
+        <f aca="false">1470* (185 + C100) / 360</f>
+        <v>386.895833333333</v>
       </c>
       <c r="E100" s="0" t="n">
         <f aca="false">735 * (90 - B100) / 180</f>
@@ -2818,8 +2819,8 @@
         <v>-2.333333</v>
       </c>
       <c r="D101" s="0" t="n">
-        <f aca="false">1470* (180 + C101) / 360</f>
-        <v>725.472223583333</v>
+        <f aca="false">1470* (185 + C101) / 360</f>
+        <v>745.88889025</v>
       </c>
       <c r="E101" s="0" t="n">
         <f aca="false">735 * (90 - B101) / 180</f>
@@ -2837,8 +2838,8 @@
         <v>-10</v>
       </c>
       <c r="D102" s="0" t="n">
-        <f aca="false">1470* (180 + C102) / 360</f>
-        <v>694.166666666667</v>
+        <f aca="false">1470* (185 + C102) / 360</f>
+        <v>714.583333333333</v>
       </c>
       <c r="E102" s="0" t="n">
         <f aca="false">735 * (90 - B102) / 180</f>
@@ -2856,8 +2857,8 @@
         <v>-15</v>
       </c>
       <c r="D103" s="0" t="n">
-        <f aca="false">1470* (180 + C103) / 360</f>
-        <v>673.75</v>
+        <f aca="false">1470* (185 + C103) / 360</f>
+        <v>694.166666666667</v>
       </c>
       <c r="E103" s="0" t="n">
         <f aca="false">735 * (90 - B103) / 180</f>
@@ -2875,8 +2876,8 @@
         <v>-59</v>
       </c>
       <c r="D104" s="0" t="n">
-        <f aca="false">1470* (180 + C104) / 360</f>
-        <v>494.083333333333</v>
+        <f aca="false">1470* (185 + C104) / 360</f>
+        <v>514.5</v>
       </c>
       <c r="E104" s="0" t="n">
         <f aca="false">735 * (90 - B104) / 180</f>
@@ -2894,8 +2895,8 @@
         <v>-72.416667</v>
       </c>
       <c r="D105" s="0" t="n">
-        <f aca="false">1470* (180 + C105) / 360</f>
-        <v>439.29860975</v>
+        <f aca="false">1470* (185 + C105) / 360</f>
+        <v>459.715276416667</v>
       </c>
       <c r="E105" s="0" t="n">
         <f aca="false">735 * (90 - B105) / 180</f>
@@ -2913,8 +2914,8 @@
         <v>73</v>
       </c>
       <c r="D106" s="0" t="n">
-        <f aca="false">1470* (180 + C106) / 360</f>
-        <v>1033.08333333333</v>
+        <f aca="false">1470* (185 + C106) / 360</f>
+        <v>1053.5</v>
       </c>
       <c r="E106" s="0" t="n">
         <f aca="false">735 * (90 - B106) / 180</f>
@@ -2932,8 +2933,8 @@
         <v>-86.5</v>
       </c>
       <c r="D107" s="0" t="n">
-        <f aca="false">1470* (180 + C107) / 360</f>
-        <v>381.791666666667</v>
+        <f aca="false">1470* (185 + C107) / 360</f>
+        <v>402.208333333333</v>
       </c>
       <c r="E107" s="0" t="n">
         <f aca="false">735 * (90 - B107) / 180</f>
@@ -2951,8 +2952,8 @@
         <v>114.166667</v>
       </c>
       <c r="D108" s="0" t="n">
-        <f aca="false">1470* (180 + C108) / 360</f>
-        <v>1201.18055691667</v>
+        <f aca="false">1470* (185 + C108) / 360</f>
+        <v>1221.59722358333</v>
       </c>
       <c r="E108" s="0" t="n">
         <f aca="false">735 * (90 - B108) / 180</f>
@@ -2970,8 +2971,8 @@
         <v>20</v>
       </c>
       <c r="D109" s="0" t="n">
-        <f aca="false">1470* (180 + C109) / 360</f>
-        <v>816.666666666667</v>
+        <f aca="false">1470* (185 + C109) / 360</f>
+        <v>837.083333333333</v>
       </c>
       <c r="E109" s="0" t="n">
         <f aca="false">735 * (90 - B109) / 180</f>
@@ -2989,8 +2990,8 @@
         <v>-18</v>
       </c>
       <c r="D110" s="0" t="n">
-        <f aca="false">1470* (180 + C110) / 360</f>
-        <v>661.5</v>
+        <f aca="false">1470* (185 + C110) / 360</f>
+        <v>681.916666666667</v>
       </c>
       <c r="E110" s="0" t="n">
         <f aca="false">735 * (90 - B110) / 180</f>
@@ -3008,8 +3009,8 @@
         <v>77</v>
       </c>
       <c r="D111" s="0" t="n">
-        <f aca="false">1470* (180 + C111) / 360</f>
-        <v>1049.41666666667</v>
+        <f aca="false">1470* (185 + C111) / 360</f>
+        <v>1069.83333333333</v>
       </c>
       <c r="E111" s="0" t="n">
         <f aca="false">735 * (90 - B111) / 180</f>
@@ -3027,8 +3028,8 @@
         <v>120</v>
       </c>
       <c r="D112" s="0" t="n">
-        <f aca="false">1470* (180 + C112) / 360</f>
-        <v>1225</v>
+        <f aca="false">1470* (185 + C112) / 360</f>
+        <v>1245.41666666667</v>
       </c>
       <c r="E112" s="0" t="n">
         <f aca="false">735 * (90 - B112) / 180</f>
@@ -3046,8 +3047,8 @@
         <v>53</v>
       </c>
       <c r="D113" s="0" t="n">
-        <f aca="false">1470* (180 + C113) / 360</f>
-        <v>951.416666666667</v>
+        <f aca="false">1470* (185 + C113) / 360</f>
+        <v>971.833333333333</v>
       </c>
       <c r="E113" s="0" t="n">
         <f aca="false">735 * (90 - B113) / 180</f>
@@ -3065,8 +3066,8 @@
         <v>44</v>
       </c>
       <c r="D114" s="0" t="n">
-        <f aca="false">1470* (180 + C114) / 360</f>
-        <v>914.666666666667</v>
+        <f aca="false">1470* (185 + C114) / 360</f>
+        <v>935.083333333333</v>
       </c>
       <c r="E114" s="0" t="n">
         <f aca="false">735 * (90 - B114) / 180</f>
@@ -3084,8 +3085,8 @@
         <v>-8</v>
       </c>
       <c r="D115" s="0" t="n">
-        <f aca="false">1470* (180 + C115) / 360</f>
-        <v>702.333333333333</v>
+        <f aca="false">1470* (185 + C115) / 360</f>
+        <v>722.75</v>
       </c>
       <c r="E115" s="0" t="n">
         <f aca="false">735 * (90 - B115) / 180</f>
@@ -3103,8 +3104,8 @@
         <v>-4.5</v>
       </c>
       <c r="D116" s="0" t="n">
-        <f aca="false">1470* (180 + C116) / 360</f>
-        <v>716.625</v>
+        <f aca="false">1470* (185 + C116) / 360</f>
+        <v>737.041666666667</v>
       </c>
       <c r="E116" s="0" t="n">
         <f aca="false">735 * (90 - B116) / 180</f>
@@ -3122,8 +3123,8 @@
         <v>34.75</v>
       </c>
       <c r="D117" s="0" t="n">
-        <f aca="false">1470* (180 + C117) / 360</f>
-        <v>876.895833333333</v>
+        <f aca="false">1470* (185 + C117) / 360</f>
+        <v>897.3125</v>
       </c>
       <c r="E117" s="0" t="n">
         <f aca="false">735 * (90 - B117) / 180</f>
@@ -3141,8 +3142,8 @@
         <v>12.833333</v>
       </c>
       <c r="D118" s="0" t="n">
-        <f aca="false">1470* (180 + C118) / 360</f>
-        <v>787.402776416667</v>
+        <f aca="false">1470* (185 + C118) / 360</f>
+        <v>807.819443083333</v>
       </c>
       <c r="E118" s="0" t="n">
         <f aca="false">735 * (90 - B118) / 180</f>
@@ -3160,8 +3161,8 @@
         <v>-77.5</v>
       </c>
       <c r="D119" s="0" t="n">
-        <f aca="false">1470* (180 + C119) / 360</f>
-        <v>418.541666666667</v>
+        <f aca="false">1470* (185 + C119) / 360</f>
+        <v>438.958333333333</v>
       </c>
       <c r="E119" s="0" t="n">
         <f aca="false">735 * (90 - B119) / 180</f>
@@ -3179,8 +3180,8 @@
         <v>138</v>
       </c>
       <c r="D120" s="0" t="n">
-        <f aca="false">1470* (180 + C120) / 360</f>
-        <v>1298.5</v>
+        <f aca="false">1470* (185 + C120) / 360</f>
+        <v>1318.91666666667</v>
       </c>
       <c r="E120" s="0" t="n">
         <f aca="false">735 * (90 - B120) / 180</f>
@@ -3198,8 +3199,8 @@
         <v>-2.116667</v>
       </c>
       <c r="D121" s="0" t="n">
-        <f aca="false">1470* (180 + C121) / 360</f>
-        <v>726.356943083333</v>
+        <f aca="false">1470* (185 + C121) / 360</f>
+        <v>746.77360975</v>
       </c>
       <c r="E121" s="0" t="n">
         <f aca="false">735 * (90 - B121) / 180</f>
@@ -3217,8 +3218,8 @@
         <v>36</v>
       </c>
       <c r="D122" s="0" t="n">
-        <f aca="false">1470* (180 + C122) / 360</f>
-        <v>882</v>
+        <f aca="false">1470* (185 + C122) / 360</f>
+        <v>902.416666666667</v>
       </c>
       <c r="E122" s="0" t="n">
         <f aca="false">735 * (90 - B122) / 180</f>
@@ -3236,8 +3237,8 @@
         <v>42.71667</v>
       </c>
       <c r="D123" s="0" t="n">
-        <f aca="false">1470* (180 + C123) / 360</f>
-        <v>909.4264025</v>
+        <f aca="false">1470* (185 + C123) / 360</f>
+        <v>929.843069166667</v>
       </c>
       <c r="E123" s="0" t="n">
         <f aca="false">735 * (90 - B123) / 180</f>
@@ -3255,8 +3256,8 @@
         <v>68</v>
       </c>
       <c r="D124" s="0" t="n">
-        <f aca="false">1470* (180 + C124) / 360</f>
-        <v>1012.66666666667</v>
+        <f aca="false">1470* (185 + C124) / 360</f>
+        <v>1033.08333333333</v>
       </c>
       <c r="E124" s="0" t="n">
         <f aca="false">735 * (90 - B124) / 180</f>
@@ -3274,8 +3275,8 @@
         <v>38</v>
       </c>
       <c r="D125" s="0" t="n">
-        <f aca="false">1470* (180 + C125) / 360</f>
-        <v>890.166666666667</v>
+        <f aca="false">1470* (185 + C125) / 360</f>
+        <v>910.583333333333</v>
       </c>
       <c r="E125" s="0" t="n">
         <f aca="false">735 * (90 - B125) / 180</f>
@@ -3293,8 +3294,8 @@
         <v>-170</v>
       </c>
       <c r="D126" s="0" t="n">
-        <f aca="false">1470* (180 + C126) / 360</f>
-        <v>40.8333333333333</v>
+        <f aca="false">1470* (185 + C126) / 360</f>
+        <v>61.25</v>
       </c>
       <c r="E126" s="0" t="n">
         <f aca="false">735 * (90 - B126) / 180</f>
@@ -3312,8 +3313,8 @@
         <v>21</v>
       </c>
       <c r="D127" s="0" t="n">
-        <f aca="false">1470* (180 + C127) / 360</f>
-        <v>820.75</v>
+        <f aca="false">1470* (185 + C127) / 360</f>
+        <v>841.166666666667</v>
       </c>
       <c r="E127" s="0" t="n">
         <f aca="false">735 * (90 - B127) / 180</f>
@@ -3331,8 +3332,8 @@
         <v>47.75</v>
       </c>
       <c r="D128" s="0" t="n">
-        <f aca="false">1470* (180 + C128) / 360</f>
-        <v>929.979166666667</v>
+        <f aca="false">1470* (185 + C128) / 360</f>
+        <v>950.395833333333</v>
       </c>
       <c r="E128" s="0" t="n">
         <f aca="false">735 * (90 - B128) / 180</f>
@@ -3350,8 +3351,8 @@
         <v>75</v>
       </c>
       <c r="D129" s="0" t="n">
-        <f aca="false">1470* (180 + C129) / 360</f>
-        <v>1041.25</v>
+        <f aca="false">1470* (185 + C129) / 360</f>
+        <v>1061.66666666667</v>
       </c>
       <c r="E129" s="0" t="n">
         <f aca="false">735 * (90 - B129) / 180</f>
@@ -3369,8 +3370,8 @@
         <v>105</v>
       </c>
       <c r="D130" s="0" t="n">
-        <f aca="false">1470* (180 + C130) / 360</f>
-        <v>1163.75</v>
+        <f aca="false">1470* (185 + C130) / 360</f>
+        <v>1184.16666666667</v>
       </c>
       <c r="E130" s="0" t="n">
         <f aca="false">735 * (90 - B130) / 180</f>
@@ -3388,8 +3389,8 @@
         <v>25</v>
       </c>
       <c r="D131" s="0" t="n">
-        <f aca="false">1470* (180 + C131) / 360</f>
-        <v>837.083333333333</v>
+        <f aca="false">1470* (185 + C131) / 360</f>
+        <v>857.5</v>
       </c>
       <c r="E131" s="0" t="n">
         <f aca="false">735 * (90 - B131) / 180</f>
@@ -3407,8 +3408,8 @@
         <v>35.833333</v>
       </c>
       <c r="D132" s="0" t="n">
-        <f aca="false">1470* (180 + C132) / 360</f>
-        <v>881.319443083333</v>
+        <f aca="false">1470* (185 + C132) / 360</f>
+        <v>901.73610975</v>
       </c>
       <c r="E132" s="0" t="n">
         <f aca="false">735 * (90 - B132) / 180</f>
@@ -3426,8 +3427,8 @@
         <v>28.25</v>
       </c>
       <c r="D133" s="0" t="n">
-        <f aca="false">1470* (180 + C133) / 360</f>
-        <v>850.354166666667</v>
+        <f aca="false">1470* (185 + C133) / 360</f>
+        <v>870.770833333333</v>
       </c>
       <c r="E133" s="0" t="n">
         <f aca="false">735 * (90 - B133) / 180</f>
@@ -3445,8 +3446,8 @@
         <v>-9.5</v>
       </c>
       <c r="D134" s="0" t="n">
-        <f aca="false">1470* (180 + C134) / 360</f>
-        <v>696.208333333333</v>
+        <f aca="false">1470* (185 + C134) / 360</f>
+        <v>716.625</v>
       </c>
       <c r="E134" s="0" t="n">
         <f aca="false">735 * (90 - B134) / 180</f>
@@ -3464,8 +3465,8 @@
         <v>17</v>
       </c>
       <c r="D135" s="0" t="n">
-        <f aca="false">1470* (180 + C135) / 360</f>
-        <v>804.416666666667</v>
+        <f aca="false">1470* (185 + C135) / 360</f>
+        <v>824.833333333333</v>
       </c>
       <c r="E135" s="0" t="n">
         <f aca="false">735 * (90 - B135) / 180</f>
@@ -3483,8 +3484,8 @@
         <v>9.533333</v>
       </c>
       <c r="D136" s="0" t="n">
-        <f aca="false">1470* (180 + C136) / 360</f>
-        <v>773.927776416667</v>
+        <f aca="false">1470* (185 + C136) / 360</f>
+        <v>794.344443083333</v>
       </c>
       <c r="E136" s="0" t="n">
         <f aca="false">735 * (90 - B136) / 180</f>
@@ -3502,8 +3503,8 @@
         <v>24</v>
       </c>
       <c r="D137" s="0" t="n">
-        <f aca="false">1470* (180 + C137) / 360</f>
-        <v>833</v>
+        <f aca="false">1470* (185 + C137) / 360</f>
+        <v>853.416666666667</v>
       </c>
       <c r="E137" s="0" t="n">
         <f aca="false">735 * (90 - B137) / 180</f>
@@ -3521,8 +3522,8 @@
         <v>6.166667</v>
       </c>
       <c r="D138" s="0" t="n">
-        <f aca="false">1470* (180 + C138) / 360</f>
-        <v>760.180556916667</v>
+        <f aca="false">1470* (185 + C138) / 360</f>
+        <v>780.597223583333</v>
       </c>
       <c r="E138" s="0" t="n">
         <f aca="false">735 * (90 - B138) / 180</f>
@@ -3540,8 +3541,8 @@
         <v>113.559722</v>
       </c>
       <c r="D139" s="0" t="n">
-        <f aca="false">1470* (180 + C139) / 360</f>
-        <v>1198.70219816667</v>
+        <f aca="false">1470* (185 + C139) / 360</f>
+        <v>1219.11886483333</v>
       </c>
       <c r="E139" s="0" t="n">
         <f aca="false">735 * (90 - B139) / 180</f>
@@ -3559,8 +3560,8 @@
         <v>22</v>
       </c>
       <c r="D140" s="0" t="n">
-        <f aca="false">1470* (180 + C140) / 360</f>
-        <v>824.833333333333</v>
+        <f aca="false">1470* (185 + C140) / 360</f>
+        <v>845.25</v>
       </c>
       <c r="E140" s="0" t="n">
         <f aca="false">735 * (90 - B140) / 180</f>
@@ -3578,8 +3579,8 @@
         <v>47</v>
       </c>
       <c r="D141" s="0" t="n">
-        <f aca="false">1470* (180 + C141) / 360</f>
-        <v>926.916666666667</v>
+        <f aca="false">1470* (185 + C141) / 360</f>
+        <v>947.333333333333</v>
       </c>
       <c r="E141" s="0" t="n">
         <f aca="false">735 * (90 - B141) / 180</f>
@@ -3597,8 +3598,8 @@
         <v>34</v>
       </c>
       <c r="D142" s="0" t="n">
-        <f aca="false">1470* (180 + C142) / 360</f>
-        <v>873.833333333333</v>
+        <f aca="false">1470* (185 + C142) / 360</f>
+        <v>894.25</v>
       </c>
       <c r="E142" s="0" t="n">
         <f aca="false">735 * (90 - B142) / 180</f>
@@ -3616,8 +3617,8 @@
         <v>112.5</v>
       </c>
       <c r="D143" s="0" t="n">
-        <f aca="false">1470* (180 + C143) / 360</f>
-        <v>1194.375</v>
+        <f aca="false">1470* (185 + C143) / 360</f>
+        <v>1214.79166666667</v>
       </c>
       <c r="E143" s="0" t="n">
         <f aca="false">735 * (90 - B143) / 180</f>
@@ -3635,8 +3636,8 @@
         <v>73</v>
       </c>
       <c r="D144" s="0" t="n">
-        <f aca="false">1470* (180 + C144) / 360</f>
-        <v>1033.08333333333</v>
+        <f aca="false">1470* (185 + C144) / 360</f>
+        <v>1053.5</v>
       </c>
       <c r="E144" s="0" t="n">
         <f aca="false">735 * (90 - B144) / 180</f>
@@ -3654,8 +3655,8 @@
         <v>-4</v>
       </c>
       <c r="D145" s="0" t="n">
-        <f aca="false">1470* (180 + C145) / 360</f>
-        <v>718.666666666667</v>
+        <f aca="false">1470* (185 + C145) / 360</f>
+        <v>739.083333333333</v>
       </c>
       <c r="E145" s="0" t="n">
         <f aca="false">735 * (90 - B145) / 180</f>
@@ -3673,8 +3674,8 @@
         <v>14.433333</v>
       </c>
       <c r="D146" s="0" t="n">
-        <f aca="false">1470* (180 + C146) / 360</f>
-        <v>793.93610975</v>
+        <f aca="false">1470* (185 + C146) / 360</f>
+        <v>814.352776416667</v>
       </c>
       <c r="E146" s="0" t="n">
         <f aca="false">735 * (90 - B146) / 180</f>
@@ -3692,8 +3693,8 @@
         <v>167</v>
       </c>
       <c r="D147" s="0" t="n">
-        <f aca="false">1470* (180 + C147) / 360</f>
-        <v>1416.91666666667</v>
+        <f aca="false">1470* (185 + C147) / 360</f>
+        <v>1437.33333333333</v>
       </c>
       <c r="E147" s="0" t="n">
         <f aca="false">735 * (90 - B147) / 180</f>
@@ -3711,8 +3712,8 @@
         <v>-61</v>
       </c>
       <c r="D148" s="0" t="n">
-        <f aca="false">1470* (180 + C148) / 360</f>
-        <v>485.916666666667</v>
+        <f aca="false">1470* (185 + C148) / 360</f>
+        <v>506.333333333333</v>
       </c>
       <c r="E148" s="0" t="n">
         <f aca="false">735 * (90 - B148) / 180</f>
@@ -3730,8 +3731,8 @@
         <v>-12</v>
       </c>
       <c r="D149" s="0" t="n">
-        <f aca="false">1470* (180 + C149) / 360</f>
-        <v>686</v>
+        <f aca="false">1470* (185 + C149) / 360</f>
+        <v>706.416666666667</v>
       </c>
       <c r="E149" s="0" t="n">
         <f aca="false">735 * (90 - B149) / 180</f>
@@ -3749,8 +3750,8 @@
         <v>57.583333</v>
       </c>
       <c r="D150" s="0" t="n">
-        <f aca="false">1470* (180 + C150) / 360</f>
-        <v>970.131943083333</v>
+        <f aca="false">1470* (185 + C150) / 360</f>
+        <v>990.54860975</v>
       </c>
       <c r="E150" s="0" t="n">
         <f aca="false">735 * (90 - B150) / 180</f>
@@ -3768,8 +3769,8 @@
         <v>45.166667</v>
       </c>
       <c r="D151" s="0" t="n">
-        <f aca="false">1470* (180 + C151) / 360</f>
-        <v>919.430556916667</v>
+        <f aca="false">1470* (185 + C151) / 360</f>
+        <v>939.847223583333</v>
       </c>
       <c r="E151" s="0" t="n">
         <f aca="false">735 * (90 - B151) / 180</f>
@@ -3787,8 +3788,8 @@
         <v>-102</v>
       </c>
       <c r="D152" s="0" t="n">
-        <f aca="false">1470* (180 + C152) / 360</f>
-        <v>318.5</v>
+        <f aca="false">1470* (185 + C152) / 360</f>
+        <v>338.916666666667</v>
       </c>
       <c r="E152" s="0" t="n">
         <f aca="false">735 * (90 - B152) / 180</f>
@@ -3806,8 +3807,8 @@
         <v>29</v>
       </c>
       <c r="D153" s="0" t="n">
-        <f aca="false">1470* (180 + C153) / 360</f>
-        <v>853.416666666667</v>
+        <f aca="false">1470* (185 + C153) / 360</f>
+        <v>873.833333333333</v>
       </c>
       <c r="E153" s="0" t="n">
         <f aca="false">735 * (90 - B153) / 180</f>
@@ -3825,8 +3826,8 @@
         <v>7.4</v>
       </c>
       <c r="D154" s="0" t="n">
-        <f aca="false">1470* (180 + C154) / 360</f>
-        <v>765.216666666667</v>
+        <f aca="false">1470* (185 + C154) / 360</f>
+        <v>785.633333333333</v>
       </c>
       <c r="E154" s="0" t="n">
         <f aca="false">735 * (90 - B154) / 180</f>
@@ -3844,8 +3845,8 @@
         <v>105</v>
       </c>
       <c r="D155" s="0" t="n">
-        <f aca="false">1470* (180 + C155) / 360</f>
-        <v>1163.75</v>
+        <f aca="false">1470* (185 + C155) / 360</f>
+        <v>1184.16666666667</v>
       </c>
       <c r="E155" s="0" t="n">
         <f aca="false">735 * (90 - B155) / 180</f>
@@ -3863,8 +3864,8 @@
         <v>19.3</v>
       </c>
       <c r="D156" s="0" t="n">
-        <f aca="false">1470* (180 + C156) / 360</f>
-        <v>813.808333333333</v>
+        <f aca="false">1470* (185 + C156) / 360</f>
+        <v>834.225</v>
       </c>
       <c r="E156" s="0" t="n">
         <f aca="false">735 * (90 - B156) / 180</f>
@@ -3882,8 +3883,8 @@
         <v>-62.2</v>
       </c>
       <c r="D157" s="0" t="n">
-        <f aca="false">1470* (180 + C157) / 360</f>
-        <v>481.016666666667</v>
+        <f aca="false">1470* (185 + C157) / 360</f>
+        <v>501.433333333333</v>
       </c>
       <c r="E157" s="0" t="n">
         <f aca="false">735 * (90 - B157) / 180</f>
@@ -3901,8 +3902,8 @@
         <v>-5</v>
       </c>
       <c r="D158" s="0" t="n">
-        <f aca="false">1470* (180 + C158) / 360</f>
-        <v>714.583333333333</v>
+        <f aca="false">1470* (185 + C158) / 360</f>
+        <v>735</v>
       </c>
       <c r="E158" s="0" t="n">
         <f aca="false">735 * (90 - B158) / 180</f>
@@ -3920,8 +3921,8 @@
         <v>35</v>
       </c>
       <c r="D159" s="0" t="n">
-        <f aca="false">1470* (180 + C159) / 360</f>
-        <v>877.916666666667</v>
+        <f aca="false">1470* (185 + C159) / 360</f>
+        <v>898.333333333333</v>
       </c>
       <c r="E159" s="0" t="n">
         <f aca="false">735 * (90 - B159) / 180</f>
@@ -3939,8 +3940,8 @@
         <v>17</v>
       </c>
       <c r="D160" s="0" t="n">
-        <f aca="false">1470* (180 + C160) / 360</f>
-        <v>804.416666666667</v>
+        <f aca="false">1470* (185 + C160) / 360</f>
+        <v>824.833333333333</v>
       </c>
       <c r="E160" s="0" t="n">
         <f aca="false">735 * (90 - B160) / 180</f>
@@ -3958,8 +3959,8 @@
         <v>166.916667</v>
       </c>
       <c r="D161" s="0" t="n">
-        <f aca="false">1470* (180 + C161) / 360</f>
-        <v>1416.57639025</v>
+        <f aca="false">1470* (185 + C161) / 360</f>
+        <v>1436.99305691667</v>
       </c>
       <c r="E161" s="0" t="n">
         <f aca="false">735 * (90 - B161) / 180</f>
@@ -3977,8 +3978,8 @@
         <v>84</v>
       </c>
       <c r="D162" s="0" t="n">
-        <f aca="false">1470* (180 + C162) / 360</f>
-        <v>1078</v>
+        <f aca="false">1470* (185 + C162) / 360</f>
+        <v>1098.41666666667</v>
       </c>
       <c r="E162" s="0" t="n">
         <f aca="false">735 * (90 - B162) / 180</f>
@@ -3996,8 +3997,8 @@
         <v>5.75</v>
       </c>
       <c r="D163" s="0" t="n">
-        <f aca="false">1470* (180 + C163) / 360</f>
-        <v>758.479166666667</v>
+        <f aca="false">1470* (185 + C163) / 360</f>
+        <v>778.895833333333</v>
       </c>
       <c r="E163" s="0" t="n">
         <f aca="false">735 * (90 - B163) / 180</f>
@@ -4015,8 +4016,8 @@
         <v>165.5</v>
       </c>
       <c r="D164" s="0" t="n">
-        <f aca="false">1470* (180 + C164) / 360</f>
-        <v>1410.79166666667</v>
+        <f aca="false">1470* (185 + C164) / 360</f>
+        <v>1431.20833333333</v>
       </c>
       <c r="E164" s="0" t="n">
         <f aca="false">735 * (90 - B164) / 180</f>
@@ -4034,8 +4035,8 @@
         <v>174</v>
       </c>
       <c r="D165" s="0" t="n">
-        <f aca="false">1470* (180 + C165) / 360</f>
-        <v>1445.5</v>
+        <f aca="false">1470* (185 + C165) / 360</f>
+        <v>1465.91666666667</v>
       </c>
       <c r="E165" s="0" t="n">
         <f aca="false">735 * (90 - B165) / 180</f>
@@ -4053,8 +4054,8 @@
         <v>-85</v>
       </c>
       <c r="D166" s="0" t="n">
-        <f aca="false">1470* (180 + C166) / 360</f>
-        <v>387.916666666667</v>
+        <f aca="false">1470* (185 + C166) / 360</f>
+        <v>408.333333333333</v>
       </c>
       <c r="E166" s="0" t="n">
         <f aca="false">735 * (90 - B166) / 180</f>
@@ -4072,8 +4073,8 @@
         <v>8</v>
       </c>
       <c r="D167" s="0" t="n">
-        <f aca="false">1470* (180 + C167) / 360</f>
-        <v>767.666666666667</v>
+        <f aca="false">1470* (185 + C167) / 360</f>
+        <v>788.083333333333</v>
       </c>
       <c r="E167" s="0" t="n">
         <f aca="false">735 * (90 - B167) / 180</f>
@@ -4091,8 +4092,8 @@
         <v>8</v>
       </c>
       <c r="D168" s="0" t="n">
-        <f aca="false">1470* (180 + C168) / 360</f>
-        <v>767.666666666667</v>
+        <f aca="false">1470* (185 + C168) / 360</f>
+        <v>788.083333333333</v>
       </c>
       <c r="E168" s="0" t="n">
         <f aca="false">735 * (90 - B168) / 180</f>
@@ -4110,8 +4111,8 @@
         <v>-169.866667</v>
       </c>
       <c r="D169" s="0" t="n">
-        <f aca="false">1470* (180 + C169) / 360</f>
-        <v>41.3777764166666</v>
+        <f aca="false">1470* (185 + C169) / 360</f>
+        <v>61.7944430833333</v>
       </c>
       <c r="E169" s="0" t="n">
         <f aca="false">735 * (90 - B169) / 180</f>
@@ -4129,8 +4130,8 @@
         <v>167.95</v>
       </c>
       <c r="D170" s="0" t="n">
-        <f aca="false">1470* (180 + C170) / 360</f>
-        <v>1420.79583333333</v>
+        <f aca="false">1470* (185 + C170) / 360</f>
+        <v>1441.2125</v>
       </c>
       <c r="E170" s="0" t="n">
         <f aca="false">735 * (90 - B170) / 180</f>
@@ -4148,8 +4149,8 @@
         <v>127</v>
       </c>
       <c r="D171" s="0" t="n">
-        <f aca="false">1470* (180 + C171) / 360</f>
-        <v>1253.58333333333</v>
+        <f aca="false">1470* (185 + C171) / 360</f>
+        <v>1274</v>
       </c>
       <c r="E171" s="0" t="n">
         <f aca="false">735 * (90 - B171) / 180</f>
@@ -4167,8 +4168,8 @@
         <v>146</v>
       </c>
       <c r="D172" s="0" t="n">
-        <f aca="false">1470* (180 + C172) / 360</f>
-        <v>1331.16666666667</v>
+        <f aca="false">1470* (185 + C172) / 360</f>
+        <v>1351.58333333333</v>
       </c>
       <c r="E172" s="0" t="n">
         <f aca="false">735 * (90 - B172) / 180</f>
@@ -4186,8 +4187,8 @@
         <v>10</v>
       </c>
       <c r="D173" s="0" t="n">
-        <f aca="false">1470* (180 + C173) / 360</f>
-        <v>775.833333333333</v>
+        <f aca="false">1470* (185 + C173) / 360</f>
+        <v>796.25</v>
       </c>
       <c r="E173" s="0" t="n">
         <f aca="false">735 * (90 - B173) / 180</f>
@@ -4205,8 +4206,8 @@
         <v>57</v>
       </c>
       <c r="D174" s="0" t="n">
-        <f aca="false">1470* (180 + C174) / 360</f>
-        <v>967.75</v>
+        <f aca="false">1470* (185 + C174) / 360</f>
+        <v>988.166666666667</v>
       </c>
       <c r="E174" s="0" t="n">
         <f aca="false">735 * (90 - B174) / 180</f>
@@ -4224,8 +4225,8 @@
         <v>70</v>
       </c>
       <c r="D175" s="0" t="n">
-        <f aca="false">1470* (180 + C175) / 360</f>
-        <v>1020.83333333333</v>
+        <f aca="false">1470* (185 + C175) / 360</f>
+        <v>1041.25</v>
       </c>
       <c r="E175" s="0" t="n">
         <f aca="false">735 * (90 - B175) / 180</f>
@@ -4243,8 +4244,8 @@
         <v>134</v>
       </c>
       <c r="D176" s="0" t="n">
-        <f aca="false">1470* (180 + C176) / 360</f>
-        <v>1282.16666666667</v>
+        <f aca="false">1470* (185 + C176) / 360</f>
+        <v>1302.58333333333</v>
       </c>
       <c r="E176" s="0" t="n">
         <f aca="false">735 * (90 - B176) / 180</f>
@@ -4262,8 +4263,8 @@
         <v>-80</v>
       </c>
       <c r="D177" s="0" t="n">
-        <f aca="false">1470* (180 + C177) / 360</f>
-        <v>408.333333333333</v>
+        <f aca="false">1470* (185 + C177) / 360</f>
+        <v>428.75</v>
       </c>
       <c r="E177" s="0" t="n">
         <f aca="false">735 * (90 - B177) / 180</f>
@@ -4281,8 +4282,8 @@
         <v>147</v>
       </c>
       <c r="D178" s="0" t="n">
-        <f aca="false">1470* (180 + C178) / 360</f>
-        <v>1335.25</v>
+        <f aca="false">1470* (185 + C178) / 360</f>
+        <v>1355.66666666667</v>
       </c>
       <c r="E178" s="0" t="n">
         <f aca="false">735 * (90 - B178) / 180</f>
@@ -4300,8 +4301,8 @@
         <v>-57.996389</v>
       </c>
       <c r="D179" s="0" t="n">
-        <f aca="false">1470* (180 + C179) / 360</f>
-        <v>498.181411583333</v>
+        <f aca="false">1470* (185 + C179) / 360</f>
+        <v>518.59807825</v>
       </c>
       <c r="E179" s="0" t="n">
         <f aca="false">735 * (90 - B179) / 180</f>
@@ -4319,8 +4320,8 @@
         <v>-76</v>
       </c>
       <c r="D180" s="0" t="n">
-        <f aca="false">1470* (180 + C180) / 360</f>
-        <v>424.666666666667</v>
+        <f aca="false">1470* (185 + C180) / 360</f>
+        <v>445.083333333333</v>
       </c>
       <c r="E180" s="0" t="n">
         <f aca="false">735 * (90 - B180) / 180</f>
@@ -4338,8 +4339,8 @@
         <v>122</v>
       </c>
       <c r="D181" s="0" t="n">
-        <f aca="false">1470* (180 + C181) / 360</f>
-        <v>1233.16666666667</v>
+        <f aca="false">1470* (185 + C181) / 360</f>
+        <v>1253.58333333333</v>
       </c>
       <c r="E181" s="0" t="n">
         <f aca="false">735 * (90 - B181) / 180</f>
@@ -4357,8 +4358,8 @@
         <v>-130.1</v>
       </c>
       <c r="D182" s="0" t="n">
-        <f aca="false">1470* (180 + C182) / 360</f>
-        <v>203.758333333333</v>
+        <f aca="false">1470* (185 + C182) / 360</f>
+        <v>224.175</v>
       </c>
       <c r="E182" s="0" t="n">
         <f aca="false">735 * (90 - B182) / 180</f>
@@ -4376,8 +4377,8 @@
         <v>20</v>
       </c>
       <c r="D183" s="0" t="n">
-        <f aca="false">1470* (180 + C183) / 360</f>
-        <v>816.666666666667</v>
+        <f aca="false">1470* (185 + C183) / 360</f>
+        <v>837.083333333333</v>
       </c>
       <c r="E183" s="0" t="n">
         <f aca="false">735 * (90 - B183) / 180</f>
@@ -4395,8 +4396,8 @@
         <v>-8</v>
       </c>
       <c r="D184" s="0" t="n">
-        <f aca="false">1470* (180 + C184) / 360</f>
-        <v>702.333333333333</v>
+        <f aca="false">1470* (185 + C184) / 360</f>
+        <v>722.75</v>
       </c>
       <c r="E184" s="0" t="n">
         <f aca="false">735 * (90 - B184) / 180</f>
@@ -4414,8 +4415,8 @@
         <v>-66.4998941</v>
       </c>
       <c r="D185" s="0" t="n">
-        <f aca="false">1470* (180 + C185) / 360</f>
-        <v>463.458765758333</v>
+        <f aca="false">1470* (185 + C185) / 360</f>
+        <v>483.875432425</v>
       </c>
       <c r="E185" s="0" t="n">
         <f aca="false">735 * (90 - B185) / 180</f>
@@ -4433,8 +4434,8 @@
         <v>51.25</v>
       </c>
       <c r="D186" s="0" t="n">
-        <f aca="false">1470* (180 + C186) / 360</f>
-        <v>944.270833333333</v>
+        <f aca="false">1470* (185 + C186) / 360</f>
+        <v>964.6875</v>
       </c>
       <c r="E186" s="0" t="n">
         <f aca="false">735 * (90 - B186) / 180</f>
@@ -4452,8 +4453,8 @@
         <v>15</v>
       </c>
       <c r="D187" s="0" t="n">
-        <f aca="false">1470* (180 + C187) / 360</f>
-        <v>796.25</v>
+        <f aca="false">1470* (185 + C187) / 360</f>
+        <v>816.666666666667</v>
       </c>
       <c r="E187" s="0" t="n">
         <f aca="false">735 * (90 - B187) / 180</f>
@@ -4471,8 +4472,8 @@
         <v>55.6</v>
       </c>
       <c r="D188" s="0" t="n">
-        <f aca="false">1470* (180 + C188) / 360</f>
-        <v>962.033333333333</v>
+        <f aca="false">1470* (185 + C188) / 360</f>
+        <v>982.45</v>
       </c>
       <c r="E188" s="0" t="n">
         <f aca="false">735 * (90 - B188) / 180</f>
@@ -4490,8 +4491,8 @@
         <v>25</v>
       </c>
       <c r="D189" s="0" t="n">
-        <f aca="false">1470* (180 + C189) / 360</f>
-        <v>837.083333333333</v>
+        <f aca="false">1470* (185 + C189) / 360</f>
+        <v>857.5</v>
       </c>
       <c r="E189" s="0" t="n">
         <f aca="false">735 * (90 - B189) / 180</f>
@@ -4509,8 +4510,8 @@
         <v>100</v>
       </c>
       <c r="D190" s="0" t="n">
-        <f aca="false">1470* (180 + C190) / 360</f>
-        <v>1143.33333333333</v>
+        <f aca="false">1470* (185 + C190) / 360</f>
+        <v>1163.75</v>
       </c>
       <c r="E190" s="0" t="n">
         <f aca="false">735 * (90 - B190) / 180</f>
@@ -4528,8 +4529,8 @@
         <v>30</v>
       </c>
       <c r="D191" s="0" t="n">
-        <f aca="false">1470* (180 + C191) / 360</f>
-        <v>857.5</v>
+        <f aca="false">1470* (185 + C191) / 360</f>
+        <v>877.916666666667</v>
       </c>
       <c r="E191" s="0" t="n">
         <f aca="false">735 * (90 - B191) / 180</f>
@@ -4547,8 +4548,8 @@
         <v>-62.833333</v>
       </c>
       <c r="D192" s="0" t="n">
-        <f aca="false">1470* (180 + C192) / 360</f>
-        <v>478.430556916667</v>
+        <f aca="false">1470* (185 + C192) / 360</f>
+        <v>498.847223583333</v>
       </c>
       <c r="E192" s="0" t="n">
         <f aca="false">735 * (90 - B192) / 180</f>
@@ -4566,8 +4567,8 @@
         <v>-62.75</v>
       </c>
       <c r="D193" s="0" t="n">
-        <f aca="false">1470* (180 + C193) / 360</f>
-        <v>478.770833333333</v>
+        <f aca="false">1470* (185 + C193) / 360</f>
+        <v>499.1875</v>
       </c>
       <c r="E193" s="0" t="n">
         <f aca="false">735 * (90 - B193) / 180</f>
@@ -4585,8 +4586,8 @@
         <v>-60.966667</v>
       </c>
       <c r="D194" s="0" t="n">
-        <f aca="false">1470* (180 + C194) / 360</f>
-        <v>486.052776416667</v>
+        <f aca="false">1470* (185 + C194) / 360</f>
+        <v>506.469443083333</v>
       </c>
       <c r="E194" s="0" t="n">
         <f aca="false">735 * (90 - B194) / 180</f>
@@ -4604,8 +4605,8 @@
         <v>-63.05833</v>
       </c>
       <c r="D195" s="0" t="n">
-        <f aca="false">1470* (180 + C195) / 360</f>
-        <v>477.511819166667</v>
+        <f aca="false">1470* (185 + C195) / 360</f>
+        <v>497.928485833333</v>
       </c>
       <c r="E195" s="0" t="n">
         <f aca="false">735 * (90 - B195) / 180</f>
@@ -4623,8 +4624,8 @@
         <v>-56.333333</v>
       </c>
       <c r="D196" s="0" t="n">
-        <f aca="false">1470* (180 + C196) / 360</f>
-        <v>504.972223583333</v>
+        <f aca="false">1470* (185 + C196) / 360</f>
+        <v>525.38889025</v>
       </c>
       <c r="E196" s="0" t="n">
         <f aca="false">735 * (90 - B196) / 180</f>
@@ -4642,8 +4643,8 @@
         <v>-61.2</v>
       </c>
       <c r="D197" s="0" t="n">
-        <f aca="false">1470* (180 + C197) / 360</f>
-        <v>485.1</v>
+        <f aca="false">1470* (185 + C197) / 360</f>
+        <v>505.516666666667</v>
       </c>
       <c r="E197" s="0" t="n">
         <f aca="false">735 * (90 - B197) / 180</f>
@@ -4661,8 +4662,8 @@
         <v>-172.178309</v>
       </c>
       <c r="D198" s="0" t="n">
-        <f aca="false">1470* (180 + C198) / 360</f>
-        <v>31.9385715833333</v>
+        <f aca="false">1470* (185 + C198) / 360</f>
+        <v>52.35523825</v>
       </c>
       <c r="E198" s="0" t="n">
         <f aca="false">735 * (90 - B198) / 180</f>
@@ -4680,8 +4681,8 @@
         <v>12.416667</v>
       </c>
       <c r="D199" s="0" t="n">
-        <f aca="false">1470* (180 + C199) / 360</f>
-        <v>785.70139025</v>
+        <f aca="false">1470* (185 + C199) / 360</f>
+        <v>806.118056916667</v>
       </c>
       <c r="E199" s="0" t="n">
         <f aca="false">735 * (90 - B199) / 180</f>
@@ -4699,8 +4700,8 @@
         <v>7</v>
       </c>
       <c r="D200" s="0" t="n">
-        <f aca="false">1470* (180 + C200) / 360</f>
-        <v>763.583333333333</v>
+        <f aca="false">1470* (185 + C200) / 360</f>
+        <v>784</v>
       </c>
       <c r="E200" s="0" t="n">
         <f aca="false">735 * (90 - B200) / 180</f>
@@ -4718,8 +4719,8 @@
         <v>45</v>
       </c>
       <c r="D201" s="0" t="n">
-        <f aca="false">1470* (180 + C201) / 360</f>
-        <v>918.75</v>
+        <f aca="false">1470* (185 + C201) / 360</f>
+        <v>939.166666666667</v>
       </c>
       <c r="E201" s="0" t="n">
         <f aca="false">735 * (90 - B201) / 180</f>
@@ -4737,8 +4738,8 @@
         <v>-14</v>
       </c>
       <c r="D202" s="0" t="n">
-        <f aca="false">1470* (180 + C202) / 360</f>
-        <v>677.833333333333</v>
+        <f aca="false">1470* (185 + C202) / 360</f>
+        <v>698.25</v>
       </c>
       <c r="E202" s="0" t="n">
         <f aca="false">735 * (90 - B202) / 180</f>
@@ -4756,8 +4757,8 @@
         <v>21</v>
       </c>
       <c r="D203" s="0" t="n">
-        <f aca="false">1470* (180 + C203) / 360</f>
-        <v>820.75</v>
+        <f aca="false">1470* (185 + C203) / 360</f>
+        <v>841.166666666667</v>
       </c>
       <c r="E203" s="0" t="n">
         <f aca="false">735 * (90 - B203) / 180</f>
@@ -4775,8 +4776,8 @@
         <v>55.666667</v>
       </c>
       <c r="D204" s="0" t="n">
-        <f aca="false">1470* (180 + C204) / 360</f>
-        <v>962.305556916667</v>
+        <f aca="false">1470* (185 + C204) / 360</f>
+        <v>982.722223583333</v>
       </c>
       <c r="E204" s="0" t="n">
         <f aca="false">735 * (90 - B204) / 180</f>
@@ -4794,8 +4795,8 @@
         <v>-11.5</v>
       </c>
       <c r="D205" s="0" t="n">
-        <f aca="false">1470* (180 + C205) / 360</f>
-        <v>688.041666666667</v>
+        <f aca="false">1470* (185 + C205) / 360</f>
+        <v>708.458333333333</v>
       </c>
       <c r="E205" s="0" t="n">
         <f aca="false">735 * (90 - B205) / 180</f>
@@ -4813,8 +4814,8 @@
         <v>103.8</v>
       </c>
       <c r="D206" s="0" t="n">
-        <f aca="false">1470* (180 + C206) / 360</f>
-        <v>1158.85</v>
+        <f aca="false">1470* (185 + C206) / 360</f>
+        <v>1179.26666666667</v>
       </c>
       <c r="E206" s="0" t="n">
         <f aca="false">735 * (90 - B206) / 180</f>
@@ -4832,8 +4833,8 @@
         <v>-63.06667</v>
       </c>
       <c r="D207" s="0" t="n">
-        <f aca="false">1470* (180 + C207) / 360</f>
-        <v>477.477764166667</v>
+        <f aca="false">1470* (185 + C207) / 360</f>
+        <v>497.894430833333</v>
       </c>
       <c r="E207" s="0" t="n">
         <f aca="false">735 * (90 - B207) / 180</f>
@@ -4851,8 +4852,8 @@
         <v>19.5</v>
       </c>
       <c r="D208" s="0" t="n">
-        <f aca="false">1470* (180 + C208) / 360</f>
-        <v>814.625</v>
+        <f aca="false">1470* (185 + C208) / 360</f>
+        <v>835.041666666667</v>
       </c>
       <c r="E208" s="0" t="n">
         <f aca="false">735 * (90 - B208) / 180</f>
@@ -4870,8 +4871,8 @@
         <v>15.166667</v>
       </c>
       <c r="D209" s="0" t="n">
-        <f aca="false">1470* (180 + C209) / 360</f>
-        <v>796.930556916667</v>
+        <f aca="false">1470* (185 + C209) / 360</f>
+        <v>817.347223583333</v>
       </c>
       <c r="E209" s="0" t="n">
         <f aca="false">735 * (90 - B209) / 180</f>
@@ -4889,8 +4890,8 @@
         <v>159</v>
       </c>
       <c r="D210" s="0" t="n">
-        <f aca="false">1470* (180 + C210) / 360</f>
-        <v>1384.25</v>
+        <f aca="false">1470* (185 + C210) / 360</f>
+        <v>1404.66666666667</v>
       </c>
       <c r="E210" s="0" t="n">
         <f aca="false">735 * (90 - B210) / 180</f>
@@ -4908,8 +4909,8 @@
         <v>48</v>
       </c>
       <c r="D211" s="0" t="n">
-        <f aca="false">1470* (180 + C211) / 360</f>
-        <v>931</v>
+        <f aca="false">1470* (185 + C211) / 360</f>
+        <v>951.416666666667</v>
       </c>
       <c r="E211" s="0" t="n">
         <f aca="false">735 * (90 - B211) / 180</f>
@@ -4927,8 +4928,8 @@
         <v>26</v>
       </c>
       <c r="D212" s="0" t="n">
-        <f aca="false">1470* (180 + C212) / 360</f>
-        <v>841.166666666667</v>
+        <f aca="false">1470* (185 + C212) / 360</f>
+        <v>861.583333333333</v>
       </c>
       <c r="E212" s="0" t="n">
         <f aca="false">735 * (90 - B212) / 180</f>
@@ -4946,8 +4947,8 @@
         <v>-33</v>
       </c>
       <c r="D213" s="0" t="n">
-        <f aca="false">1470* (180 + C213) / 360</f>
-        <v>600.25</v>
+        <f aca="false">1470* (185 + C213) / 360</f>
+        <v>620.666666666667</v>
       </c>
       <c r="E213" s="0" t="n">
         <f aca="false">735 * (90 - B213) / 180</f>
@@ -4965,8 +4966,8 @@
         <v>127.5</v>
       </c>
       <c r="D214" s="0" t="n">
-        <f aca="false">1470* (180 + C214) / 360</f>
-        <v>1255.625</v>
+        <f aca="false">1470* (185 + C214) / 360</f>
+        <v>1276.04166666667</v>
       </c>
       <c r="E214" s="0" t="n">
         <f aca="false">735 * (90 - B214) / 180</f>
@@ -4984,8 +4985,8 @@
         <v>30</v>
       </c>
       <c r="D215" s="0" t="n">
-        <f aca="false">1470* (180 + C215) / 360</f>
-        <v>857.5</v>
+        <f aca="false">1470* (185 + C215) / 360</f>
+        <v>877.916666666667</v>
       </c>
       <c r="E215" s="0" t="n">
         <f aca="false">735 * (90 - B215) / 180</f>
@@ -5003,8 +5004,8 @@
         <v>-4</v>
       </c>
       <c r="D216" s="0" t="n">
-        <f aca="false">1470* (180 + C216) / 360</f>
-        <v>718.666666666667</v>
+        <f aca="false">1470* (185 + C216) / 360</f>
+        <v>739.083333333333</v>
       </c>
       <c r="E216" s="0" t="n">
         <f aca="false">735 * (90 - B216) / 180</f>
@@ -5022,8 +5023,8 @@
         <v>81</v>
       </c>
       <c r="D217" s="0" t="n">
-        <f aca="false">1470* (180 + C217) / 360</f>
-        <v>1065.75</v>
+        <f aca="false">1470* (185 + C217) / 360</f>
+        <v>1086.16666666667</v>
       </c>
       <c r="E217" s="0" t="n">
         <f aca="false">735 * (90 - B217) / 180</f>
@@ -5041,8 +5042,8 @@
         <v>30</v>
       </c>
       <c r="D218" s="0" t="n">
-        <f aca="false">1470* (180 + C218) / 360</f>
-        <v>857.5</v>
+        <f aca="false">1470* (185 + C218) / 360</f>
+        <v>877.916666666667</v>
       </c>
       <c r="E218" s="0" t="n">
         <f aca="false">735 * (90 - B218) / 180</f>
@@ -5060,8 +5061,8 @@
         <v>-56</v>
       </c>
       <c r="D219" s="0" t="n">
-        <f aca="false">1470* (180 + C219) / 360</f>
-        <v>506.333333333333</v>
+        <f aca="false">1470* (185 + C219) / 360</f>
+        <v>526.75</v>
       </c>
       <c r="E219" s="0" t="n">
         <f aca="false">735 * (90 - B219) / 180</f>
@@ -5079,8 +5080,8 @@
         <v>20</v>
       </c>
       <c r="D220" s="0" t="n">
-        <f aca="false">1470* (180 + C220) / 360</f>
-        <v>816.666666666667</v>
+        <f aca="false">1470* (185 + C220) / 360</f>
+        <v>837.083333333333</v>
       </c>
       <c r="E220" s="0" t="n">
         <f aca="false">735 * (90 - B220) / 180</f>
@@ -5098,8 +5099,8 @@
         <v>31.5</v>
       </c>
       <c r="D221" s="0" t="n">
-        <f aca="false">1470* (180 + C221) / 360</f>
-        <v>863.625</v>
+        <f aca="false">1470* (185 + C221) / 360</f>
+        <v>884.041666666667</v>
       </c>
       <c r="E221" s="0" t="n">
         <f aca="false">735 * (90 - B221) / 180</f>
@@ -5117,8 +5118,8 @@
         <v>15</v>
       </c>
       <c r="D222" s="0" t="n">
-        <f aca="false">1470* (180 + C222) / 360</f>
-        <v>796.25</v>
+        <f aca="false">1470* (185 + C222) / 360</f>
+        <v>816.666666666667</v>
       </c>
       <c r="E222" s="0" t="n">
         <f aca="false">735 * (90 - B222) / 180</f>
@@ -5136,8 +5137,8 @@
         <v>8</v>
       </c>
       <c r="D223" s="0" t="n">
-        <f aca="false">1470* (180 + C223) / 360</f>
-        <v>767.666666666667</v>
+        <f aca="false">1470* (185 + C223) / 360</f>
+        <v>788.083333333333</v>
       </c>
       <c r="E223" s="0" t="n">
         <f aca="false">735 * (90 - B223) / 180</f>
@@ -5155,8 +5156,8 @@
         <v>38</v>
       </c>
       <c r="D224" s="0" t="n">
-        <f aca="false">1470* (180 + C224) / 360</f>
-        <v>890.166666666667</v>
+        <f aca="false">1470* (185 + C224) / 360</f>
+        <v>910.583333333333</v>
       </c>
       <c r="E224" s="0" t="n">
         <f aca="false">735 * (90 - B224) / 180</f>
@@ -5174,8 +5175,8 @@
         <v>121</v>
       </c>
       <c r="D225" s="0" t="n">
-        <f aca="false">1470* (180 + C225) / 360</f>
-        <v>1229.08333333333</v>
+        <f aca="false">1470* (185 + C225) / 360</f>
+        <v>1249.5</v>
       </c>
       <c r="E225" s="0" t="n">
         <f aca="false">735 * (90 - B225) / 180</f>
@@ -5193,8 +5194,8 @@
         <v>71</v>
       </c>
       <c r="D226" s="0" t="n">
-        <f aca="false">1470* (180 + C226) / 360</f>
-        <v>1024.91666666667</v>
+        <f aca="false">1470* (185 + C226) / 360</f>
+        <v>1045.33333333333</v>
       </c>
       <c r="E226" s="0" t="n">
         <f aca="false">735 * (90 - B226) / 180</f>
@@ -5212,8 +5213,8 @@
         <v>35</v>
       </c>
       <c r="D227" s="0" t="n">
-        <f aca="false">1470* (180 + C227) / 360</f>
-        <v>877.916666666667</v>
+        <f aca="false">1470* (185 + C227) / 360</f>
+        <v>898.333333333333</v>
       </c>
       <c r="E227" s="0" t="n">
         <f aca="false">735 * (90 - B227) / 180</f>
@@ -5231,8 +5232,8 @@
         <v>100</v>
       </c>
       <c r="D228" s="0" t="n">
-        <f aca="false">1470* (180 + C228) / 360</f>
-        <v>1143.33333333333</v>
+        <f aca="false">1470* (185 + C228) / 360</f>
+        <v>1163.75</v>
       </c>
       <c r="E228" s="0" t="n">
         <f aca="false">735 * (90 - B228) / 180</f>
@@ -5250,8 +5251,8 @@
         <v>125.75</v>
       </c>
       <c r="D229" s="0" t="n">
-        <f aca="false">1470* (180 + C229) / 360</f>
-        <v>1248.47916666667</v>
+        <f aca="false">1470* (185 + C229) / 360</f>
+        <v>1268.89583333333</v>
       </c>
       <c r="E229" s="0" t="n">
         <f aca="false">735 * (90 - B229) / 180</f>
@@ -5269,8 +5270,8 @@
         <v>1.166667</v>
       </c>
       <c r="D230" s="0" t="n">
-        <f aca="false">1470* (180 + C230) / 360</f>
-        <v>739.76389025</v>
+        <f aca="false">1470* (185 + C230) / 360</f>
+        <v>760.180556916667</v>
       </c>
       <c r="E230" s="0" t="n">
         <f aca="false">735 * (90 - B230) / 180</f>
@@ -5288,8 +5289,8 @@
         <v>-171.75</v>
       </c>
       <c r="D231" s="0" t="n">
-        <f aca="false">1470* (180 + C231) / 360</f>
-        <v>33.6875</v>
+        <f aca="false">1470* (185 + C231) / 360</f>
+        <v>54.1041666666667</v>
       </c>
       <c r="E231" s="0" t="n">
         <f aca="false">735 * (90 - B231) / 180</f>
@@ -5307,8 +5308,8 @@
         <v>-175</v>
       </c>
       <c r="D232" s="0" t="n">
-        <f aca="false">1470* (180 + C232) / 360</f>
-        <v>20.4166666666667</v>
+        <f aca="false">1470* (185 + C232) / 360</f>
+        <v>40.8333333333333</v>
       </c>
       <c r="E232" s="0" t="n">
         <f aca="false">735 * (90 - B232) / 180</f>
@@ -5326,8 +5327,8 @@
         <v>-61</v>
       </c>
       <c r="D233" s="0" t="n">
-        <f aca="false">1470* (180 + C233) / 360</f>
-        <v>485.916666666667</v>
+        <f aca="false">1470* (185 + C233) / 360</f>
+        <v>506.333333333333</v>
       </c>
       <c r="E233" s="0" t="n">
         <f aca="false">735 * (90 - B233) / 180</f>
@@ -5345,8 +5346,8 @@
         <v>54.416667</v>
       </c>
       <c r="D234" s="0" t="n">
-        <f aca="false">1470* (180 + C234) / 360</f>
-        <v>957.20139025</v>
+        <f aca="false">1470* (185 + C234) / 360</f>
+        <v>977.618056916667</v>
       </c>
       <c r="E234" s="0" t="n">
         <f aca="false">735 * (90 - B234) / 180</f>
@@ -5364,8 +5365,8 @@
         <v>9</v>
       </c>
       <c r="D235" s="0" t="n">
-        <f aca="false">1470* (180 + C235) / 360</f>
-        <v>771.75</v>
+        <f aca="false">1470* (185 + C235) / 360</f>
+        <v>792.166666666667</v>
       </c>
       <c r="E235" s="0" t="n">
         <f aca="false">735 * (90 - B235) / 180</f>
@@ -5383,8 +5384,8 @@
         <v>34.911546</v>
       </c>
       <c r="D236" s="0" t="n">
-        <f aca="false">1470* (180 + C236) / 360</f>
-        <v>877.5554795</v>
+        <f aca="false">1470* (185 + C236) / 360</f>
+        <v>897.972146166667</v>
       </c>
       <c r="E236" s="0" t="n">
         <f aca="false">735 * (90 - B236) / 180</f>
@@ -5402,8 +5403,8 @@
         <v>60</v>
       </c>
       <c r="D237" s="0" t="n">
-        <f aca="false">1470* (180 + C237) / 360</f>
-        <v>980</v>
+        <f aca="false">1470* (185 + C237) / 360</f>
+        <v>1000.41666666667</v>
       </c>
       <c r="E237" s="0" t="n">
         <f aca="false">735 * (90 - B237) / 180</f>
@@ -5421,8 +5422,8 @@
         <v>-71.583333</v>
       </c>
       <c r="D238" s="0" t="n">
-        <f aca="false">1470* (180 + C238) / 360</f>
-        <v>442.70139025</v>
+        <f aca="false">1470* (185 + C238) / 360</f>
+        <v>463.118056916667</v>
       </c>
       <c r="E238" s="0" t="n">
         <f aca="false">735 * (90 - B238) / 180</f>
@@ -5440,8 +5441,8 @@
         <v>178</v>
       </c>
       <c r="D239" s="0" t="n">
-        <f aca="false">1470* (180 + C239) / 360</f>
-        <v>1461.83333333333</v>
+        <f aca="false">1470* (185 + C239) / 360</f>
+        <v>1482.25</v>
       </c>
       <c r="E239" s="0" t="n">
         <f aca="false">735 * (90 - B239) / 180</f>
@@ -5459,8 +5460,8 @@
         <v>33</v>
       </c>
       <c r="D240" s="0" t="n">
-        <f aca="false">1470* (180 + C240) / 360</f>
-        <v>869.75</v>
+        <f aca="false">1470* (185 + C240) / 360</f>
+        <v>890.166666666667</v>
       </c>
       <c r="E240" s="0" t="n">
         <f aca="false">735 * (90 - B240) / 180</f>
@@ -5478,8 +5479,8 @@
         <v>32</v>
       </c>
       <c r="D241" s="0" t="n">
-        <f aca="false">1470* (180 + C241) / 360</f>
-        <v>865.666666666667</v>
+        <f aca="false">1470* (185 + C241) / 360</f>
+        <v>886.083333333333</v>
       </c>
       <c r="E241" s="0" t="n">
         <f aca="false">735 * (90 - B241) / 180</f>
@@ -5497,8 +5498,8 @@
         <v>54</v>
       </c>
       <c r="D242" s="0" t="n">
-        <f aca="false">1470* (180 + C242) / 360</f>
-        <v>955.5</v>
+        <f aca="false">1470* (185 + C242) / 360</f>
+        <v>975.916666666667</v>
       </c>
       <c r="E242" s="0" t="n">
         <f aca="false">735 * (90 - B242) / 180</f>
@@ -5516,8 +5517,8 @@
         <v>-4</v>
       </c>
       <c r="D243" s="0" t="n">
-        <f aca="false">1470* (180 + C243) / 360</f>
-        <v>718.666666666667</v>
+        <f aca="false">1470* (185 + C243) / 360</f>
+        <v>739.083333333333</v>
       </c>
       <c r="E243" s="0" t="n">
         <f aca="false">735 * (90 - B243) / 180</f>
@@ -5535,8 +5536,8 @@
         <v>-98.5795</v>
       </c>
       <c r="D244" s="0" t="n">
-        <f aca="false">1470* (180 + C244) / 360</f>
-        <v>332.467041666667</v>
+        <f aca="false">1470* (185 + C244) / 360</f>
+        <v>352.883708333333</v>
       </c>
       <c r="E244" s="0" t="n">
         <f aca="false">735 * (90 - B244) / 180</f>
@@ -5554,8 +5555,8 @@
         <v>-56</v>
       </c>
       <c r="D245" s="0" t="n">
-        <f aca="false">1470* (180 + C245) / 360</f>
-        <v>506.333333333333</v>
+        <f aca="false">1470* (185 + C245) / 360</f>
+        <v>526.75</v>
       </c>
       <c r="E245" s="0" t="n">
         <f aca="false">735 * (90 - B245) / 180</f>
@@ -5573,8 +5574,8 @@
         <v>-162.0725</v>
       </c>
       <c r="D246" s="0" t="n">
-        <f aca="false">1470* (180 + C246) / 360</f>
-        <v>73.2039583333334</v>
+        <f aca="false">1470* (185 + C246) / 360</f>
+        <v>93.620625</v>
       </c>
       <c r="E246" s="0" t="n">
         <f aca="false">735 * (90 - B246) / 180</f>
@@ -5592,8 +5593,8 @@
         <v>-64.9834807</v>
       </c>
       <c r="D247" s="0" t="n">
-        <f aca="false">1470* (180 + C247) / 360</f>
-        <v>469.650787141667</v>
+        <f aca="false">1470* (185 + C247) / 360</f>
+        <v>490.067453808333</v>
       </c>
       <c r="E247" s="0" t="n">
         <f aca="false">735 * (90 - B247) / 180</f>
@@ -5611,8 +5612,8 @@
         <v>63.84911</v>
       </c>
       <c r="D248" s="0" t="n">
-        <f aca="false">1470* (180 + C248) / 360</f>
-        <v>995.717199166667</v>
+        <f aca="false">1470* (185 + C248) / 360</f>
+        <v>1016.13386583333</v>
       </c>
       <c r="E248" s="0" t="n">
         <f aca="false">735 * (90 - B248) / 180</f>
@@ -5630,8 +5631,8 @@
         <v>167</v>
       </c>
       <c r="D249" s="0" t="n">
-        <f aca="false">1470* (180 + C249) / 360</f>
-        <v>1416.91666666667</v>
+        <f aca="false">1470* (185 + C249) / 360</f>
+        <v>1437.33333333333</v>
       </c>
       <c r="E249" s="0" t="n">
         <f aca="false">735 * (90 - B249) / 180</f>
@@ -5649,8 +5650,8 @@
         <v>12.45</v>
       </c>
       <c r="D250" s="0" t="n">
-        <f aca="false">1470* (180 + C250) / 360</f>
-        <v>785.8375</v>
+        <f aca="false">1470* (185 + C250) / 360</f>
+        <v>806.254166666667</v>
       </c>
       <c r="E250" s="0" t="n">
         <f aca="false">735 * (90 - B250) / 180</f>
@@ -5668,8 +5669,8 @@
         <v>-66</v>
       </c>
       <c r="D251" s="0" t="n">
-        <f aca="false">1470* (180 + C251) / 360</f>
-        <v>465.5</v>
+        <f aca="false">1470* (185 + C251) / 360</f>
+        <v>485.916666666667</v>
       </c>
       <c r="E251" s="0" t="n">
         <f aca="false">735 * (90 - B251) / 180</f>
@@ -5687,8 +5688,8 @@
         <v>107.833333</v>
       </c>
       <c r="D252" s="0" t="n">
-        <f aca="false">1470* (180 + C252) / 360</f>
-        <v>1175.31944308333</v>
+        <f aca="false">1470* (185 + C252) / 360</f>
+        <v>1195.73610975</v>
       </c>
       <c r="E252" s="0" t="n">
         <f aca="false">735 * (90 - B252) / 180</f>
@@ -5706,8 +5707,8 @@
         <v>-176.2</v>
       </c>
       <c r="D253" s="0" t="n">
-        <f aca="false">1470* (180 + C253) / 360</f>
-        <v>15.5166666666667</v>
+        <f aca="false">1470* (185 + C253) / 360</f>
+        <v>35.9333333333334</v>
       </c>
       <c r="E253" s="0" t="n">
         <f aca="false">735 * (90 - B253) / 180</f>
@@ -5725,8 +5726,8 @@
         <v>35.25</v>
       </c>
       <c r="D254" s="0" t="n">
-        <f aca="false">1470* (180 + C254) / 360</f>
-        <v>878.9375</v>
+        <f aca="false">1470* (185 + C254) / 360</f>
+        <v>899.354166666667</v>
       </c>
       <c r="E254" s="0" t="n">
         <f aca="false">735 * (90 - B254) / 180</f>
@@ -5744,8 +5745,8 @@
         <v>-13.5</v>
       </c>
       <c r="D255" s="0" t="n">
-        <f aca="false">1470* (180 + C255) / 360</f>
-        <v>679.875</v>
+        <f aca="false">1470* (185 + C255) / 360</f>
+        <v>700.291666666667</v>
       </c>
       <c r="E255" s="0" t="n">
         <f aca="false">735 * (90 - B255) / 180</f>
@@ -5763,8 +5764,8 @@
         <v>47.5</v>
       </c>
       <c r="D256" s="0" t="n">
-        <f aca="false">1470* (180 + C256) / 360</f>
-        <v>928.958333333333</v>
+        <f aca="false">1470* (185 + C256) / 360</f>
+        <v>949.375</v>
       </c>
       <c r="E256" s="0" t="n">
         <f aca="false">735 * (90 - B256) / 180</f>
@@ -5782,8 +5783,8 @@
         <v>30</v>
       </c>
       <c r="D257" s="0" t="n">
-        <f aca="false">1470* (180 + C257) / 360</f>
-        <v>857.5</v>
+        <f aca="false">1470* (185 + C257) / 360</f>
+        <v>877.916666666667</v>
       </c>
       <c r="E257" s="0" t="n">
         <f aca="false">735 * (90 - B257) / 180</f>
@@ -5801,8 +5802,8 @@
         <v>29</v>
       </c>
       <c r="D258" s="0" t="n">
-        <f aca="false">1470* (180 + C258) / 360</f>
-        <v>853.416666666667</v>
+        <f aca="false">1470* (185 + C258) / 360</f>
+        <v>873.833333333333</v>
       </c>
       <c r="E258" s="0" t="n">
         <f aca="false">735 * (90 - B258) / 180</f>

</xml_diff>